<commit_message>
Started to write the code to put the two pieces of code together in the temp file
</commit_message>
<xml_diff>
--- a/product_reviews.xlsx
+++ b/product_reviews.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>product</t>
   </si>
@@ -37,187 +37,112 @@
     <t>body</t>
   </si>
   <si>
-    <t>Sony WH-CH510 Wireless Bluetooth Headphones with Mic, 35 Hours Battery Life with Quick Charge, On-ear Style, Hands-Free Call, Voice Assistant - Black</t>
-  </si>
-  <si>
-    <t>Full review and durability test</t>
-  </si>
-  <si>
-    <t>Pretty Good</t>
-  </si>
-  <si>
-    <t>3 Weeks In... I'm Impressed!</t>
-  </si>
-  <si>
-    <t>Subpar at most</t>
-  </si>
-  <si>
-    <t>Best in class</t>
-  </si>
-  <si>
-    <t>Good all round. But not amazing.</t>
-  </si>
-  <si>
-    <t>great for self isolation with the husband</t>
-  </si>
-  <si>
-    <t>I have cheaper headphones that do the same job...</t>
-  </si>
-  <si>
-    <t>Uncomfortable head strap and terrible microphone feedback mar what could have been a good product</t>
-  </si>
-  <si>
-    <t>Best headphones I've ever had!</t>
+    <t>LEGO 42123 Technic McLaren Senna GTR Racing Sports Collectable Model Car, Vehicle Toy Construction Set, Idea</t>
+  </si>
+  <si>
+    <t>You'll be happy to build this</t>
+  </si>
+  <si>
+    <t>Mindless fun to escape reality</t>
+  </si>
+  <si>
+    <t>Brilliant model</t>
+  </si>
+  <si>
+    <t>Good beginner set, now im hooked</t>
+  </si>
+  <si>
+    <t>Complex enough to be a challenge, but a sensible time to build</t>
+  </si>
+  <si>
+    <t>Great model, but a little fiddly.</t>
+  </si>
+  <si>
+    <t>Brilliant build quality for my 7yo</t>
+  </si>
+  <si>
+    <t>Best value for money Lego Technic car available</t>
+  </si>
+  <si>
+    <t>Superb</t>
+  </si>
+  <si>
+    <t>Great model</t>
   </si>
   <si>
     <t>Great value</t>
   </si>
   <si>
-    <t>Great value for money, typical sony sound quality</t>
-  </si>
-  <si>
-    <t>Comfortable Headset</t>
-  </si>
-  <si>
-    <t>Sidetone function problem</t>
-  </si>
-  <si>
-    <t>Good headphones.</t>
-  </si>
-  <si>
-    <t>Greatest experience of my life so far!</t>
-  </si>
-  <si>
-    <t>I LOVE THEM</t>
-  </si>
-  <si>
-    <t>Great headphones but they have one bad thing</t>
-  </si>
-  <si>
-    <t>Overpriced</t>
-  </si>
-  <si>
-    <t>Reasonably Good for the price.</t>
-  </si>
-  <si>
-    <t>Really good</t>
-  </si>
-  <si>
-    <t>Pleased</t>
-  </si>
-  <si>
-    <t>Voice is good.</t>
-  </si>
-  <si>
-    <t>Not great</t>
-  </si>
-  <si>
-    <t>Recommended</t>
-  </si>
-  <si>
-    <t>Too much re-pairing</t>
-  </si>
-  <si>
-    <t>Much better than earpods for hearing impairment</t>
-  </si>
-  <si>
-    <t>Reliable, Easy To Use, Great Battery Life</t>
-  </si>
-  <si>
-    <t>Definitely improves the viewing and listening experience</t>
-  </si>
-  <si>
-    <t>Decent Headphones for the Price</t>
-  </si>
-  <si>
-    <t>This is the first time I had been sent a product before it was publicly released in order to write a review, so I felt it only right to do a thorough product analysis. Below I have left a pros on cons list with explanations for each point.Pros:Sound - The sound is excellent, no two ways about it, no static, no hum and no muffling. It sounded sharp and clear for music, videos and telephone conversations.Microphone - This headset allows you to do hands free calls with it's built in, internal, microphone. Due to the microphone being inside the right ear drum I was worried that my voice would sound quiet but, according to the person on the other side of the phone, it doesn't sound any different from a normal phone call.Glasses - You'll have no problem wearing glasses while sporting the headset. It doesn't cause any pinching or squeezing.Light-weight - It's surprisingly light. Most wireless headsets have a bit of heft to them but, this one, I can imagine carry around without worrying about getting tired.Durable - With it's size and weight I was worried that it wouldn't be able to survive falling off someone head. So in order to find out I dropped it onto a hardwood floor from about 6 ft, twice, and was pleasantly surprised that not only did it survive but didn't have a mark on it.Cons:Little sound cancelling - It does very little to stop noise from escaping or entering. I found that while playing music the people around me could hear what I was playing if I had my volume at around 50%, I could also hear most things that were going on around me.Size - It's quite small, which can be a good thing, but I found the ear pads weren't able to cover my ears (Which may be while there's little sound cancelling). I had a female friend try them and she found that it was actually a tad too big, causing the pads to hang a bit low on her head.No head padding - Usually you'll find a pad on arch on the headset to add comfort, but not on this headset. I found the hard plastic very uncomfortable. However someone else I had wear the headset didn't mind the lack of pad, so I guess it'll depend on your head shape.Small charging cable - This is a small quibble but the charger that came in the box is remarkable small. It's a standard C charger port so this won't be a problem for most people.Overall it's not perfect, but for the current selling price of £50 I think you'll get more than your monies worth.</t>
-  </si>
-  <si>
-    <t>I have tried a multitude of headphones over the years everything from JVC, Sony, Sennheiser, Philips, WeSC to Grado, Bang &amp; Olufsen and everything in-between. For my money, Grado makes the very best over-ear headphones I have ever bought and they also have exemplary after-sales service. I received these Sony headphones and they are the sixth Sony's I have tested. I have tested the 1000 M3's to a set which retailed over £200 which were designed for Hi Fidelity and now these. From the packaging to the actual product they are nice quality and the sound they produce, given the price, is very good.The big problem in rating headphones and earbuds is that the sound they produce and how they sound is very subjective to review, as two people can listen to a piece of music but they can hear that piece of music differently. In light of this, I am going to try and be as objective about these Earphones as I can.Let us start this review by considering the price, £49.99 at the time of review. This is a good price given the quality of what you are given. They are extremely well made. Everything from the box to the headpiece appears to be top quality., given the low price The headphones themselves are made of quality materials and are quite light. What is not good is that there is no cushioning on the headband. They are not that comfortable to wear over a long period, as I have a large head and need some cushioning.The sound they produce is very good given the price. The reproduction is rich and clear, the bass is fantastic, the middle range is clear and defined and the treble is delightful. The only downside to these phones is the bass, it just lacks a bit of depth.I was not expecting great things from these headphones, yet what they give you in terms of sound quality is very good, given the price. To summarise, these headphones are very well made and produce a sound that is very good. They offer value far beyond the price point. Where they are let down is in the noise-cancelling department. These phones are designed to be used on the go. The amount of background noise is, therefore, going to be loud. This set has no noise-cancelling system and so it kind of defeats the purpose of the set. You have to ask yourself, do you need NC as you journey around? If you don't need it, these are pretty good headphones for the price.</t>
-  </si>
-  <si>
-    <t>I wanted to wait a few weeks so I could give a fair review.I must say I am impressed with these headphones!To give a bit of background, these are the first set of wireless headphones I have owned. Previous to that I owned a pair of wired Sony headphones, similar to these. I love my music, and really enjoy listening to good quality sound.My initial impressions on the headphones are good. They feel very sturdy and I love how the ear cups twist so that the headphones can be stored flat in my rucksack.Connection to Bluetooth was very quick and easy, and I was able to start listening to Spotify on my phone within 2 minutes!After a full charge overnight, I was intreiged to see how long the headphones would actually last, given the advertised 35 hour battery life!Whilst I haven't kept a diary persay, as a minimum I use the headphones for at least 4 hours a day on my commute to and from work. Each time you turn the headphones on, you have a battery notice played to you, as well as a battery indicator shown on my phone. The headphones lasted for around 7 or 8 days before the headphones advised me to recharge. I haven't run the headphones right down flat, but I would say the 35 hour life is very accurate.These are on ear headphones so it would be unreasonable to expect complete noise cancelling. I wanted a pair of headphones that would not deaden my surroundings completely as I think it's important you aren't completely unaware. However I would say the headphones cancel noise enough to be able to hear the music.I occasionally use the headphones to make and receive telephone calls, both in the office at my desk and whilst commuting. The quality is fantastic, and I've not experienced any problems with the person on the other end not being able to hear me - big thumbs up for this feature!Thinking about the reviews I saw before buying these headphones, I will do my best to remember them and give my own thoughts.- The volume of the headphones are too low, even on the highest setting.I saw a few reviews saying this, both on amazon and a few other sources. I have personally not had any issues with the volume (or lack of) on these headphones. My music taste is varied, and even the softer genres play just fine for me. It may be worth noting that there are two volumes to adjust, your phone and the headphones themselves. Depending on the device you may also be able to adjust the graphic equaliser somewhat if needed.- The headphones are too tight on my headThere has only been one occasion where I have experienced a bit of pain on my one ear, however I think they were ill-fitted as I adjusted them on my ears and they were fine thereafter. I would say I have an average sized head! I think you have to bear in mind that these headphones sit on your ears, so they will compress somewhat, so they stay on your head.I would not want them to be looser as I would be conscious they would slide around and potentially fall off my head.Some have suggested that the band itself is uncomfortable, again, I've not had any issues with this regard.All in all I think these are a really great set of headphones for the price.If your a more serious music listener then you may want to consider an alternative option, but I would consider these suitable for most!</t>
-  </si>
-  <si>
-    <t>Bought the black version, for WFH, have some support calls.- First issue is the comfort, this is not comfortable at all. The cushion goes on top of your ears and hurts after a while.- The sound is nothing remarkable, noise cancelling is non-existent. Not that I was expecting something different for this price range.Now the real issues:- When having a call, I can hear my voice, the quality of the sound drops and it really makes very hard to understand what is going on.- The real reason I'm making this review is because now I tried with two machines (Windows and Mac) and I realised the device disconnects itself from the bluetooth randomly, is like the headphone restarts itself, disconnects from the bluetooth, tells me the battery and then connects again. This has happened three times in two different machines. Note that once this was IN THE MIDDLE OF A SUPPORT CALL.Hope this goes to the manufacturer.</t>
-  </si>
-  <si>
-    <t>Perfect for a low cost Bluetooth headphones, clear sound, NOT nfc so works with my laptop, smartphone &amp; smart TV. Fairly big battery, lasts me 3/4days usage. Bluetooth connection is very good, some dropout when moving around (about 5m from device). Sleek minimalist design, very light too and comfy. Far superior to JVC equivalent.</t>
-  </si>
-  <si>
-    <t>Just a short review for any potential buyers that are unsure.Generally I’m happy with these headphones, but wish I had the patience to shop round.The look is smart and clean, with a textured finish which works for me as I mainly use them in a gym. However they do feel cheap. An all plastic finish and the ear pieces are loose and moves easily, almost too easily.They have a good fit and are snug. I’d imagine they would eventually get warm on the ears as they’re on-ear rather than over-ear.Sound quality is average. I’ve have marked them at £30-40 headphones. Good amount of bass but not particularly crisp mid and high ends. £50 seems steep. I was slightly underwhelmed - but contradictorily I’m sure I’ll like them and put them through their paces.</t>
-  </si>
-  <si>
-    <t>The husband has been working from home all week since we both have covid; sharing the same space has been hard. I have had to stay quiet all day while he is on conference call meetings. After a week of staring at the walls all day I decided to buy these. They are a bit fiddly  to connect to our LG smart tv, but it is the tv being difficult, not the headphones. the sound is good, no lag when watching sky Q/netflix. i am able to use my usb C charger to charge these which is nice. They work good for what i need them for and don't cost a fortune fyi i am a loyal sony headphone customer for many years, as others are too expensive or inferior quality, and they need to keep up with my rugged lifestyle</t>
-  </si>
-  <si>
-    <t>Edit after 5months:cheap plastic, it is already extremely loose, does not stay in place._________I am using them right now so i will review with some pros and consPRO-Sound is ok, loud enough, decent bass:-Very ligh-like the movement and the fact that on the neck, the headset can be twisted 90deg- paring is quite quickCONS-when on a phone call, there is a tremendous echo (that other mentioned). Nothing that can be done.It will also amplifies sounds from the background such an ambulance, people talkin, or your colleague sipping a smoothie..-no foam on the head-to change a song you have to press for 2.5 secs and if you use them for long distance running, it is not practical at all</t>
-  </si>
-  <si>
-    <t>I don't know what I was expecting from this headset, I didn't expect audiophile sound, or premium build quality, but I wasn't expecting an unpadded hard plastic head strap that digs into my head, is uncomfortable within a minute and unbearable within 10!I ended up wrapping the headset strap in bubble wrap until a third party strap cover arrived, and that was another tenner I shouldn't have had to budget for.Sound quality as headphones is Ok, about what I'd expect at this price point, but the microphone has incredibly irritating feedback. I wasn't expecting it it to be as good a noise cancelling headset, but the microphone picks up the headphone output, which it echoes back a fraction of a second later, causing a feedback loop. This makes it sound like you're in a cave as soon as you switch from headphone to headset mode.I wanted on-ear headphones as my ears over heat in over-ear headphones, but these clamp with enough force that even the soft leatherette pad start to get hot and uncomfortable after not too long.Charging is also irritating. It tells you how much charge is left when you turn it on, which is useful if it's low, but it would be more useful for it to tell you the charge when you turn it off. Since you can't use this headset while charging, it would be useful to know that it's worth putting them on to charge while you don't need to use them, rather than only finding out you need to charge them when you do want to use them.Overall these were very disappointing given the well respected brand. They were obviously made to a price point, but some of these problems would be so easy to fix. A few pennies for strap padding, a few more for a microphone jack port, a few more for a power management IC which allowed use while charging, these could have rounded off the worst rough edges of this product.</t>
-  </si>
-  <si>
-    <t>One of the best purchases of the lockdown. Having noisy children and still having to have those virtual meetings, I'm very pleased with this! Also amazing for listening to music as it has good bass and the sound is very clear. Yes, I don't know much of technical features and all those specific jargon people use to describe headphones, but for the others like me that only want a good product without having to sell a kidney, this is a fantastic purchase! And being wireless is a surplus, especially when you're cooking the kids lunch and still can listen to that webinar playing on your laptop because everyone knows that webinars from 11 am to 1 pm is the perfect timing to throw one! Speaking of which, they have such an amazing battery life! They last so long. Take today, for instance. They are saying low battery since yesterday and I forgot to charge them overnight and yes, they're still going for 3 hours now. One overnight charging lasts me for around 15 days, using about 10 hours a day. Very good!</t>
-  </si>
-  <si>
-    <t>I went for this headphones because of the reasonable price and good reviews. They're lightweight and comfortable but not very sturdy.  The sound is quite good especially considering the price. It was very easy to connect and they're easy to use. Overall quite happy with it, if you're looking for an inexpensive option look no further.</t>
-  </si>
-  <si>
-    <t>Very pleased with these at £35 they are amazing, typical great sony sound quality! I wanted headphones without noise cancalling as i use them around the house when doing jobs and if the other half or kids and calling or talking i wanted to hear them, i can hear them making noise but its hard to understand until i turn the volume down a bit which is very easy with buttons on the ear piece. Pretty comfy, i wasnt expecting ultimate luxury for this price so very happy with them.</t>
-  </si>
-  <si>
-    <t>I do use this headset for hours at a time (I love audiobooks). My only wrinkle is if I want to link this to multiple devices it really struggles with this so its best to just connect to one device at a time which is a shame but a minor thing really. The battery lasts for a long time I can use it all day and I do. Highly recommended.</t>
-  </si>
-  <si>
-    <t>The main problem is the Sidetone function that you cannot disable. It sends all the noise from the environment surrounding you back to you. Thus you hear everything including your voice twice. It is impossible to disable it. Thus, the mic is not useful at all.===I set the rating to 5 stars as this headphones are much better than others I tried recently with similar price.</t>
-  </si>
-  <si>
-    <t>These are very nice comfortable headphones.Bluetooth works fine.I didn't know they were supposed to have noise cancellation.  If they do, it doesn't work very well.</t>
-  </si>
-  <si>
-    <t>I have recently bought 2 of these headphones, one for me and one as a birthday gift. However, this second pair ended up going to my father - who is completely deaf in his right ear and profoundly deaf in the other. These headphones have amplified his hearing on his left to the point that he can hear even the smallest of things like paper rustling or me typing on the keyboard when we call. He is a huge music lover and has managed to hear melodies and sub-melodies he never know existed, and can finally comprehend the lyrics in complete full clarity. I truly believe this to be the best purchase I have ever made due to the knock-on effect it had, even though these headphones are amazing by themselves.</t>
-  </si>
-  <si>
-    <t>i previously had a pair on Sony wired headphones, i decided on these as i have started running and thought these would come in handy. These are fab, they connected to my phone without a problem and within a minute i was listening to my audiobook. i can sit and relax listening to these now and go running with these not slipping at all and no wire hanging. Glad i made this purchase.</t>
-  </si>
-  <si>
-    <t>So when you make a call using them even on PC you can hear your self which is so annoying and worse yet there is no way to disable that option because its designed to do that on purpose. I cant even begin to understand how stupid this is and why it even exist but other then this they are great headphones work well last long.</t>
-  </si>
-  <si>
-    <t>I thought these were overpriced for what they are, wireless plastic headphones, they do however have a pleasing baseline on the ear. I would not buy these again for a replacement, I would choose a different maker and a more expensive model.I think these were overpriced and should retail for £20 less than the asking price.</t>
-  </si>
-  <si>
-    <t>I live about 30 miles from my son but with these headphones connected to our iPhones via Bluetooth my son and I can use WhatsApp over Wi-fi to talk whilst we ride together on Zwift.Had reservations about the microphone being integral to one of the earphones but need not have worried as it picks up everything.Comfortable enough for an hour or so.Sound quality when listening to music better than I expected for the price.They don’t fall off while I’m riding and neither do I.</t>
-  </si>
-  <si>
-    <t>Amazing and totally worth the price! Cheap and quite literally the best</t>
-  </si>
-  <si>
-    <t>As with all Sony products, satisfied</t>
-  </si>
-  <si>
-    <t>Good product.</t>
-  </si>
-  <si>
-    <t>Not what expected</t>
-  </si>
-  <si>
-    <t>I bought these reasonably priced headphones to use with my phone/watch to listen to a range of music (folk/classical) and lecturers on the music. So far, I am very pleased. At this price, one cannot expect very high quality sound but they have pleased me listening to full orchestral classical pieces, small ensembles, folk duos, soloists and lectures.Not as comfortable for long periods (or as high quality sound) as my Bowers and Wilkins but these are cabled and cost over four times as much.The Sony are light, generally comfortable and link very easily with Bluetooth; the speakers voice reassuringly states the battery states and that Bluetooth has been connected (or shutdown after source turned off) and the battery life has been very good so far. Charged over night usually, there has never been an issue with the battery so far. Marked “L” and “R” with the on/off, plus minus sound controls on the right, they take a little getting used to as it is easy to misadjust but not really an issue.At this price and for all their benefits, I recommend them.</t>
-  </si>
-  <si>
-    <t>Use these with an iPod Touch 7th gen. Music playback is fine, no discernible background hiss. Nice volume range. As long as music is playing they stay connected and there are no issues. However, if I need to take a break (pause playback) or the current playlist ends;  even for a minute or two, I find I have to turn the headphones off, else the connection breaks and they switch off. When I switch them back on they do not always reconnect to the source and in some cases I actually need to re-pair the headphones to the iPod.</t>
-  </si>
-  <si>
-    <t>I replaced the bluetooth earpods because  couldnt hear clearly &amp; everytime I walked out of the room the bluetooth disconnected. I am really pleased with my headphones, very clear sound &amp; because they are wireless I dont lose my connection</t>
-  </si>
-  <si>
-    <t>I recently bought another set of cheaper Bluetooth headphones in a sale (I didn't want to keep switching pairing between my PC and my Phone on these ones). It made me appreciate how good the Sony ones are. Easy to use, built solidly and with great sound quality. I'm going to have to order another set to replace my cheap ones.</t>
-  </si>
-  <si>
-    <t>Brilliant , easy to connect , sound quality good. The up and down volume controls would have been better if they had been protruding slightly making  them easier to locate. They are flush with the on off</t>
-  </si>
-  <si>
-    <t>The headphones are easy to connect, they can be adjusted to fit different head sizes. the sound is good but not the best, bass is not as good but for the price they are a decent set of headphones, just don't expect too much from them.</t>
+    <t>Great value, good build and interesting features</t>
+  </si>
+  <si>
+    <t>Excellent item</t>
+  </si>
+  <si>
+    <t>Worth the money</t>
+  </si>
+  <si>
+    <t>Bought as a gift - very happy</t>
+  </si>
+  <si>
+    <t>Quality Stuff</t>
+  </si>
+  <si>
+    <t>Fantastic price</t>
+  </si>
+  <si>
+    <t>Fine</t>
+  </si>
+  <si>
+    <t>A very nice set to make, numbered bags are also a really big help, for the price it's a really good set</t>
+  </si>
+  <si>
+    <t>I build them, my son plays with them. Generally how it goes. He's love to build them, but he's young and struggles with his hands, so putting the pins in are a challenge (for most of us). The build quality is excellent and my son pushes around everywhere without anything falling off (I'd hate to work out where a stray piece has come from!). I only buy these when on offer though, I find spending excessive amounts of lego to be outside of my interest.</t>
+  </si>
+  <si>
+    <t>Thoroughly enjoyed making this car. It is sufficiently demanding to make it a worthwhile task. I went wrong a couple of times, which meant a bit of dismantling. However, got there in the end and it makes a great display model. Difficulty is keeping young probing fingers away. Highly recommended and a saving on price at Amazon.</t>
+  </si>
+  <si>
+    <t>My first technic set and my first lego set since i was 14 or so (31 now) and enjoyed this throughout.A not too complex set but at the same time still clever. Took around 3 hours to do the whole thing and i would say only one but frustrated me which involved the piece 6282140 (Pin with Friction Ridges Lengthwise and Pin Hole) as its hard to push them into a hole whilst they also spin around which was for the windscreen frame near the end.Overall i enjoyed this and am hooked on building again. Only complaint is lots of stickers which im not great at but tweezers helped.</t>
+  </si>
+  <si>
+    <t>I'd say this kit hits the sweet spot of a decent price, a complex enough kit to be interesting and a sensible amount of time to build. The beautiful technic car kits at north of £100-200 are magnificent pieces of work, but they are also a significant financial and time commitment. This one is a generation ahead of the £18 Speed Champions kits, but only costs twice as much, so you get much more for your money. There are some nice touches like steering and an animated V8 engine, but it doesn't extend to proper gearbox, differential and suspension like the top kits do. That said it's a great medium level kit and very good looking when complete and looks something roughly like 1/12 scale, so it doesn't take up as much shelf space as the really big car kits.</t>
+  </si>
+  <si>
+    <t>Lego isn't cheap, but for around £30 this, in my opinion, offers good value for money.A high part count, coupled with decent instructions (although they could be clearer in places) produces a lovely looking finished product.I do get a little annoyed at Lego's propensity for producing new pieces for specific shapes rather than using multiple existing parts to get the same result.  Somehow, it takes away from the challenge I experienced many years ago with the very first technical lego kits.</t>
+  </si>
+  <si>
+    <t>This was bought for a birthday present from my 7yo son to his Daddy for them to do together, but my son ended up doing it all himself - he absolutely loved it! He loves Lego Technics builds and did this one in 3/4 sittings, even getting up early before school to do it, he enjoyed it so much. Some technics kits are very expensive so this was great value for money and my son loved doing it and now plays with the finished product.</t>
+  </si>
+  <si>
+    <t>Pros- Extremely good value for money when you break down how many pieces you get compared to how much the set costs- The stickers that come with the product are unique, and make the finished product look very premium compared to other Lego products- The colour scheme is great.Cons:- It's lego, so compared to other brick products the value for money isn't that high. But you are paying for a superior product.Overall: This makes the product look great as a display piece once it's done, and it's enjoyable to build it with just the right amount of parts.</t>
+  </si>
+  <si>
+    <t>Great little build that my son thoroughly enjoyed. Quite a few stickers (46), but even at 10 he managed well with them.</t>
+  </si>
+  <si>
+    <t>I love the working pistons in the engine. Had fun with my 9yr old kid building it.  I do wish the parts were screen printed rather than stickers, but I know that's an unrealistic wish really, it's just something that bugs me with all Lego models.</t>
+  </si>
+  <si>
+    <t>Bought this for my son at university as a surprise during lockdown, he was over the moon and said that it made his week. He really appreciated it, had to build it straight away.</t>
+  </si>
+  <si>
+    <t>Great build and good looking model. With moving eight cylinder pistons, rack and pinion steering (like in my Lego Technic forklift truck about 40 years ago) and opening gull-wing doors. A bit ambitious for my nearly 8 year-old, who chose this with some Christmas money (and hardly any traditional stud-brick building)- but I enjoyed “helping” him, and he loves the end product.</t>
+  </si>
+  <si>
+    <t>Purchased for my 21yr old son who still enjoys building lego cars to wind down from a hard days at work!  This only took him a couple of hours to complete, however I imagine for someone much younger it could be spread out over a longer period of time (to get your moneys worth!)</t>
+  </si>
+  <si>
+    <t>This is a nice bit of kit and worth the money .if technic lego collector and buying your first .buy it</t>
+  </si>
+  <si>
+    <t>Really good quality and well worth the money,</t>
+  </si>
+  <si>
+    <t>Fun build and good display piece</t>
+  </si>
+  <si>
+    <t>Good fun, enjoyable experience.</t>
   </si>
 </sst>
 </file>
@@ -579,7 +504,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -619,16 +544,16 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>564</v>
+        <v>6</v>
       </c>
       <c r="F2" s="2">
-        <v>43732</v>
+        <v>44194</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -642,16 +567,16 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>175</v>
+        <v>2</v>
       </c>
       <c r="F3" s="2">
-        <v>43734</v>
+        <v>44315</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -665,16 +590,16 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>92</v>
+        <v>3</v>
       </c>
       <c r="F4" s="2">
-        <v>43801</v>
+        <v>44333</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -688,16 +613,16 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>43937</v>
+        <v>44500</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -711,16 +636,16 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="F6" s="2">
-        <v>43769</v>
+        <v>44430</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -734,16 +659,16 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="F7" s="2">
-        <v>43846</v>
+        <v>44463</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -760,13 +685,13 @@
         <v>5</v>
       </c>
       <c r="E8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F8" s="2">
-        <v>43923</v>
+        <v>44468</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -780,16 +705,16 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E9">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2">
-        <v>43887</v>
+        <v>44407</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -803,16 +728,16 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F10" s="2">
         <v>44220</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -829,13 +754,13 @@
         <v>5</v>
       </c>
       <c r="E11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2">
-        <v>44000</v>
+        <v>44301</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -849,16 +774,16 @@
         <v>2</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12" s="2">
-        <v>44450</v>
+        <v>44296</v>
       </c>
       <c r="G12" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -875,13 +800,13 @@
         <v>5</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F13" s="2">
-        <v>44093</v>
+        <v>44195</v>
       </c>
       <c r="G13" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -901,10 +826,10 @@
         <v>0</v>
       </c>
       <c r="F14" s="2">
-        <v>44256</v>
+        <v>44419</v>
       </c>
       <c r="G14" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -924,10 +849,10 @@
         <v>0</v>
       </c>
       <c r="F15" s="2">
-        <v>44214</v>
+        <v>44198</v>
       </c>
       <c r="G15" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -941,16 +866,16 @@
         <v>2</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="2">
-        <v>44336</v>
+        <v>44268</v>
       </c>
       <c r="G16" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -970,10 +895,10 @@
         <v>0</v>
       </c>
       <c r="F17" s="2">
-        <v>44403</v>
+        <v>44256</v>
       </c>
       <c r="G17" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -993,10 +918,10 @@
         <v>0</v>
       </c>
       <c r="F18" s="2">
-        <v>44216</v>
+        <v>44258</v>
       </c>
       <c r="G18" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1016,286 +941,10 @@
         <v>0</v>
       </c>
       <c r="F19" s="2">
-        <v>44373</v>
+        <v>44213</v>
       </c>
       <c r="G19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20" s="2">
-        <v>44227</v>
-      </c>
-      <c r="G20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21">
-        <v>4</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2">
-        <v>44413</v>
-      </c>
-      <c r="G21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22">
-        <v>5</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22" s="2">
-        <v>44251</v>
-      </c>
-      <c r="G22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="D23">
-        <v>5</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23" s="2">
-        <v>44271</v>
-      </c>
-      <c r="G23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
-      <c r="D24">
-        <v>5</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24" s="2">
-        <v>44250</v>
-      </c>
-      <c r="G24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25" s="2">
-        <v>44227</v>
-      </c>
-      <c r="G25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26">
-        <v>3</v>
-      </c>
-      <c r="D26">
-        <v>5</v>
-      </c>
-      <c r="E26">
-        <v>2</v>
-      </c>
-      <c r="F26" s="2">
-        <v>44043</v>
-      </c>
-      <c r="G26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="D27">
-        <v>3</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27" s="2">
-        <v>43813</v>
-      </c>
-      <c r="G27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28">
-        <v>3</v>
-      </c>
-      <c r="D28">
-        <v>5</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28" s="2">
-        <v>44294</v>
-      </c>
-      <c r="G28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29">
-        <v>3</v>
-      </c>
-      <c r="D29">
-        <v>5</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29" s="2">
-        <v>44115</v>
-      </c>
-      <c r="G29" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30">
-        <v>3</v>
-      </c>
-      <c r="D30">
-        <v>5</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30" s="2">
-        <v>44270</v>
-      </c>
-      <c r="G30" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31">
-        <v>3</v>
-      </c>
-      <c r="D31">
-        <v>3</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31" s="2">
-        <v>44231</v>
-      </c>
-      <c r="G31" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a file to play around with how to write line by line with pandas. Don't think it's possible. Also fixed a bug in composing the url which caused it to scrape page 1234 instead of 4. I've left the debugging print statements in to remind me how I fixed it. Will remove in next commit.
</commit_message>
<xml_diff>
--- a/product_reviews.xlsx
+++ b/product_reviews.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="178">
   <si>
     <t>product</t>
   </si>
@@ -70,28 +70,229 @@
     <t>Great model</t>
   </si>
   <si>
-    <t>Great value</t>
-  </si>
-  <si>
-    <t>Great value, good build and interesting features</t>
-  </si>
-  <si>
-    <t>Excellent item</t>
-  </si>
-  <si>
-    <t>Worth the money</t>
-  </si>
-  <si>
-    <t>Bought as a gift - very happy</t>
-  </si>
-  <si>
-    <t>Quality Stuff</t>
-  </si>
-  <si>
-    <t>Fantastic price</t>
-  </si>
-  <si>
-    <t>Fine</t>
+    <t>Loved lego technic</t>
+  </si>
+  <si>
+    <t>Fun and technical to build.</t>
+  </si>
+  <si>
+    <t>Lego Technic fans will love it</t>
+  </si>
+  <si>
+    <t>Good quality kit</t>
+  </si>
+  <si>
+    <t>Good quality</t>
+  </si>
+  <si>
+    <t>Competitive price and great task for The Boys / Dad and Son</t>
+  </si>
+  <si>
+    <t>A great product &amp; great value</t>
+  </si>
+  <si>
+    <t>Looks great</t>
+  </si>
+  <si>
+    <t>My 7 year old grandson loves it</t>
+  </si>
+  <si>
+    <t>It's lego it's technic</t>
+  </si>
+  <si>
+    <t>As always a lego kit delivers</t>
+  </si>
+  <si>
+    <t>Perfect Lego as always</t>
+  </si>
+  <si>
+    <t>Senna</t>
+  </si>
+  <si>
+    <t>Missing part halts build</t>
+  </si>
+  <si>
+    <t>very difficult for a clever 6 year old sadly</t>
+  </si>
+  <si>
+    <t>Looks Great</t>
+  </si>
+  <si>
+    <t>Great after all it’s Lego</t>
+  </si>
+  <si>
+    <t>Looks great assembled</t>
+  </si>
+  <si>
+    <t>Perfect for all petrolheads!</t>
+  </si>
+  <si>
+    <t>Stickers</t>
+  </si>
+  <si>
+    <t>Given as a gift</t>
+  </si>
+  <si>
+    <t>Excellent kit</t>
+  </si>
+  <si>
+    <t>birthday</t>
+  </si>
+  <si>
+    <t>Looks awesome, good value for money</t>
+  </si>
+  <si>
+    <t>Excellent Value</t>
+  </si>
+  <si>
+    <t>Fun project</t>
+  </si>
+  <si>
+    <t>Great item great price</t>
+  </si>
+  <si>
+    <t>Good price</t>
+  </si>
+  <si>
+    <t>Senna car</t>
+  </si>
+  <si>
+    <t>Technic McLaren</t>
+  </si>
+  <si>
+    <t>Lego</t>
+  </si>
+  <si>
+    <t>NICE BUILD,NICE MODEL, RECOMMENDED.</t>
+  </si>
+  <si>
+    <t>A good build!</t>
+  </si>
+  <si>
+    <t>Fun and challenging</t>
+  </si>
+  <si>
+    <t>Brilliant</t>
+  </si>
+  <si>
+    <t>Gift for dad</t>
+  </si>
+  <si>
+    <t>Great little one</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Great value for money</t>
+  </si>
+  <si>
+    <t>Perfect lego</t>
+  </si>
+  <si>
+    <t>Great gift</t>
+  </si>
+  <si>
+    <t>Excellent</t>
+  </si>
+  <si>
+    <t>A nice little build :)</t>
+  </si>
+  <si>
+    <t>Great build</t>
+  </si>
+  <si>
+    <t>damaged box</t>
+  </si>
+  <si>
+    <t>Very fun to assemble</t>
+  </si>
+  <si>
+    <t>A must for any McLaren enthusiast!</t>
+  </si>
+  <si>
+    <t>An interesting Project</t>
+  </si>
+  <si>
+    <t>Usual Amazon</t>
+  </si>
+  <si>
+    <t>Like</t>
+  </si>
+  <si>
+    <t>Car goes broom</t>
+  </si>
+  <si>
+    <t>great present for older boys too :)</t>
+  </si>
+  <si>
+    <t>All parts are there... Plus a few extra bits.</t>
+  </si>
+  <si>
+    <t>LEGO Technic is the best range of LEGO products</t>
+  </si>
+  <si>
+    <t>Great car fiddly build</t>
+  </si>
+  <si>
+    <t>Love it</t>
+  </si>
+  <si>
+    <t>McLaren Senna GTR</t>
+  </si>
+  <si>
+    <t>Great to build always enjoy Lego.</t>
+  </si>
+  <si>
+    <t>Ideal gift</t>
+  </si>
+  <si>
+    <t>Cool car</t>
+  </si>
+  <si>
+    <t>Opened and used product missing parts</t>
+  </si>
+  <si>
+    <t>It's just a great set to build</t>
+  </si>
+  <si>
+    <t>12+ would be better</t>
+  </si>
+  <si>
+    <t>Great price for what you get</t>
+  </si>
+  <si>
+    <t>Brilliant value 4 the money</t>
+  </si>
+  <si>
+    <t>WAS EASY TO ASSEMBLE</t>
+  </si>
+  <si>
+    <t>McLean  car</t>
+  </si>
+  <si>
+    <t>Son loved it</t>
+  </si>
+  <si>
+    <t>Good Quality.</t>
+  </si>
+  <si>
+    <t>Great product</t>
+  </si>
+  <si>
+    <t>Great addition to any collection</t>
+  </si>
+  <si>
+    <t>A great present</t>
+  </si>
+  <si>
+    <t>Make sure you get the right component as many are very simular</t>
+  </si>
+  <si>
+    <t>Fun to Build</t>
+  </si>
+  <si>
+    <t>Great</t>
   </si>
   <si>
     <t>A very nice set to make, numbered bags are also a really big help, for the price it's a really good set</t>
@@ -124,25 +325,229 @@
     <t>I love the working pistons in the engine. Had fun with my 9yr old kid building it.  I do wish the parts were screen printed rather than stickers, but I know that's an unrealistic wish really, it's just something that bugs me with all Lego models.</t>
   </si>
   <si>
-    <t>Bought this for my son at university as a surprise during lockdown, he was over the moon and said that it made his week. He really appreciated it, had to build it straight away.</t>
-  </si>
-  <si>
-    <t>Great build and good looking model. With moving eight cylinder pistons, rack and pinion steering (like in my Lego Technic forklift truck about 40 years ago) and opening gull-wing doors. A bit ambitious for my nearly 8 year-old, who chose this with some Christmas money (and hardly any traditional stud-brick building)- but I enjoyed “helping” him, and he loves the end product.</t>
-  </si>
-  <si>
-    <t>Purchased for my 21yr old son who still enjoys building lego cars to wind down from a hard days at work!  This only took him a couple of hours to complete, however I imagine for someone much younger it could be spread out over a longer period of time (to get your moneys worth!)</t>
-  </si>
-  <si>
-    <t>This is a nice bit of kit and worth the money .if technic lego collector and buying your first .buy it</t>
-  </si>
-  <si>
-    <t>Really good quality and well worth the money,</t>
-  </si>
-  <si>
-    <t>Fun build and good display piece</t>
-  </si>
-  <si>
-    <t>Good fun, enjoyable experience.</t>
+    <t>Loved lego technic as young kids back in the day lol and decided to purchase the Mclaren car during lockdown. Best 4.5 hours spent in a long time and brought so many childhood memories</t>
+  </si>
+  <si>
+    <t>Great product and a lot of fun to put it together! Had a lot of fun building this. Was challenging enough but not too difficult. Car looks great finished 👌</t>
+  </si>
+  <si>
+    <t>Bought for my lego-mad husband. He was so happy to get it. Standard Lego Technic quality and usually for a better price than Lego themselves sell them for.</t>
+  </si>
+  <si>
+    <t>This was bought as a present. It was quite challenging to assemble but fitted together well and all the pieces were there. The recipient was happy with it.</t>
+  </si>
+  <si>
+    <t>Very happy. Adult recipient who I gifted this too was really impressed. They said for the price it was great quality and was fun to make.</t>
+  </si>
+  <si>
+    <t>Great LEGO Technic item</t>
+  </si>
+  <si>
+    <t>I hadn’t played with Lego since I was kid, so I wanted to start off small. This car is ideal for starting out. The instructions are clear to follow and it took me a few hours to complete. The build quality is of a high standard and it’s a decent size once built as well. Highly recommend this product to anyone and the price is amazing. I will be buying more in the near future</t>
+  </si>
+  <si>
+    <t>Bought for my sons birthday, he’s not opened it yet but we have had a few others like this that have been great. Delivered on time.</t>
+  </si>
+  <si>
+    <t>Bought as a gift for my grandson who was staying at my house for a few days and he loved it. Built in a day but he is very good with Lego.</t>
+  </si>
+  <si>
+    <t>Quality lego construction, negatives, it's not instantly recognisable, and it sits a bit too high on the wheels, apart from that an enjoyable set to build</t>
+  </si>
+  <si>
+    <t>Another quality Lego model, an enjoyable build. I also managed to buy it when it was at a discounted price, so result !</t>
+  </si>
+  <si>
+    <t>This is a challenging build for adults as well as children. The final build is very impressive and sturdy - as you would expect from Lego. Great value for money too.</t>
+  </si>
+  <si>
+    <t>Absolutely brilliant.  Don't care about what anyone says but I love it. It's senna so you can't argue with that.</t>
+  </si>
+  <si>
+    <t>Unhappy with a missing axle, lego shops don’t stick. Ordered replacement from lego..still waiting.</t>
+  </si>
+  <si>
+    <t>I thought his father might help but he lost interest early on but some nice engineering features</t>
+  </si>
+  <si>
+    <t>A good  Technic to get you started into the world of Lego, easy to assemble excellent price</t>
+  </si>
+  <si>
+    <t>My teenage son loves Lego and this is no exception. Great fun to build and a decent size on completion.</t>
+  </si>
+  <si>
+    <t>Arrived on time well packagedNot so easy for a 12 year old to assemble by himself</t>
+  </si>
+  <si>
+    <t>I bought this for man who was recuperating from accident, kept him occupied for hours!!!</t>
+  </si>
+  <si>
+    <t>There are quite a few stickers but it does look good. For the money this is great value.</t>
+  </si>
+  <si>
+    <t>Bought as a gift for grandson's birthday, I haven't heard any complaints yet</t>
+  </si>
+  <si>
+    <t>Excellent kit with good instructions.Also looks fantastic when built</t>
+  </si>
+  <si>
+    <t>my grandson was very happy to receive the lego Technic Mc Laren Senna GTR</t>
+  </si>
+  <si>
+    <t>Easy to assemble, intresting build, one of my sons favourites to date.</t>
+  </si>
+  <si>
+    <t>This looks amazing &amp; for the price is an excellent addition to my collection. Who does t love Lego &amp; this was exactly what I needed to be able to chill out &amp; relax.</t>
+  </si>
+  <si>
+    <t>Great fun, looks cool and was great to build. Didn’t realise there was scaling based sections in the instructions for 1:1 ratios.</t>
+  </si>
+  <si>
+    <t>Wanted this for a gift  much cheaper than in Lego shop</t>
+  </si>
+  <si>
+    <t>Looks fantastic . Can't wait to give to grandson in Aug. 2021</t>
+  </si>
+  <si>
+    <t>On time, sure I’m going to have a very happy Grandson.</t>
+  </si>
+  <si>
+    <t>Some fiddly bits ,youngsters will need help,otherwise,good 🤩</t>
+  </si>
+  <si>
+    <t>Bought for 7 year old grandson - he loves it 👍</t>
+  </si>
+  <si>
+    <t>Bought as a gift and very much appreciated</t>
+  </si>
+  <si>
+    <t>NO COMPLAINTS&lt; VERY HAPPY WITH PURCHASE.</t>
+  </si>
+  <si>
+    <t>Bought for a Lego fan in self isolation to relieve boredom. Deffo helped!</t>
+  </si>
+  <si>
+    <t>My 15 year old was well happy with this</t>
+  </si>
+  <si>
+    <t>Excellent Lego set, well designed and accurately represented. A challenge but not too difficult.</t>
+  </si>
+  <si>
+    <t>Really enjoyed putting this together, took a couple of hours , great piece when finished, looking forward to another build</t>
+  </si>
+  <si>
+    <t>Present for my dad , he was very happy !</t>
+  </si>
+  <si>
+    <t>Another really nice Lego set. I have a couple of the bigger ones, but this new Lego car was really fun to build. Super satisfied by the final result.</t>
+  </si>
+  <si>
+    <t>Bought as present for 9 year old very happy so all good</t>
+  </si>
+  <si>
+    <t>Great gift for Lego fans.</t>
+  </si>
+  <si>
+    <t>A more interesting build than I was expecting.</t>
+  </si>
+  <si>
+    <t>Took me about 2 hours or so to complete this build. Amazing value considering the size and complexity of the set. Combines two great loves of mine, Lego and Racing Cars!</t>
+  </si>
+  <si>
+    <t>The product arrived in quicker time that estimated, but the box itself was slightly damaged on osidene of the corners and also on one of the sides, but this did not affect the contents of the box.</t>
+  </si>
+  <si>
+    <t>Very fun to assemble, my boyfriend found it easy and amusing. Good conditions.</t>
+  </si>
+  <si>
+    <t>Great addition to the collection, great job by McLaren and LEGO</t>
+  </si>
+  <si>
+    <t>It looks good.It was given as a present and a challenge to the recipient due to the number of parts it was received very well and completed in good time.Unable to access feature rating below</t>
+  </si>
+  <si>
+    <t>Is good</t>
+  </si>
+  <si>
+    <t>My kid loves it, but the price has reduced compared to when I’ve brought it.</t>
+  </si>
+  <si>
+    <t>If your buying for your kids. Good luck. If your a teenager or adult. This is great fun just remember to follow the instructions as it can be rarther confusing at times.</t>
+  </si>
+  <si>
+    <t>arrived super fast too</t>
+  </si>
+  <si>
+    <t>I took me about 1 to 13 hours to complete this, great for getting into Zen mode.</t>
+  </si>
+  <si>
+    <t>LEGO Tehnic is an interesting range that gives you the possibility to develop your creative building skills. Unfortunately this product has only one model that can be built.</t>
+  </si>
+  <si>
+    <t>Great looking model but some of the pieces were just to fiddly</t>
+  </si>
+  <si>
+    <t>As a lego lover, I love investing my time in building different models. This Mclaren Sienna model is one of my favorite and is definitely worth the price:)</t>
+  </si>
+  <si>
+    <t>Thanks 🤩 Excellent design and kept me occupied for several days doing the assembly good fun and very interesting 👍👍</t>
+  </si>
+  <si>
+    <t>It fits on my Lego car transporter perfectly.</t>
+  </si>
+  <si>
+    <t>Great for lego and car fans.</t>
+  </si>
+  <si>
+    <t>Nice set with easy to follow instructions and a good build time for the price, definitely good value for money. But so so many stickers to put on</t>
+  </si>
+  <si>
+    <t>Very dissatisfied - given to my son as a birthday present - box looked like it had been opened - car half made - definitely used.Very upset son.</t>
+  </si>
+  <si>
+    <t>10 year old struggled in certain areas, but after been helped with a bit of encouragement he loved it !!!</t>
+  </si>
+  <si>
+    <t>For the price point you get to make a surprisingly large model that’s brilliant to build and display after.</t>
+  </si>
+  <si>
+    <t>Haven't done lego 4 over 20 yrs!!! This was fun and enjoyable 2 do. Definitely going 2 get some more</t>
+  </si>
+  <si>
+    <t>ENJOYED MAKING UP THIS CAR</t>
+  </si>
+  <si>
+    <t>A very enjoyed this productNice and easy to assemble a very good product you should buy</t>
+  </si>
+  <si>
+    <t>Was present for my grandson and he loved it</t>
+  </si>
+  <si>
+    <t>My son loved building this</t>
+  </si>
+  <si>
+    <t>Easy to assemble but took six hours</t>
+  </si>
+  <si>
+    <t>A must for any Lego fan and great value for the money.</t>
+  </si>
+  <si>
+    <t>It kept my daughter quiet for days whilst she built it</t>
+  </si>
+  <si>
+    <t>A fantastic build and great addition to any collection</t>
+  </si>
+  <si>
+    <t>The final outcome a model showing how the car works and the detail</t>
+  </si>
+  <si>
+    <t>Easy to assemble, and a good price for the size</t>
+  </si>
+  <si>
+    <t>The Lego set was quite tricky to build but I managed to do it</t>
+  </si>
+  <si>
+    <t>Christmas present sorted</t>
   </si>
 </sst>
 </file>
@@ -504,7 +909,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -553,7 +958,7 @@
         <v>44194</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -576,7 +981,7 @@
         <v>44315</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -599,7 +1004,7 @@
         <v>44333</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -622,7 +1027,7 @@
         <v>44500</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -645,7 +1050,7 @@
         <v>44430</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -668,7 +1073,7 @@
         <v>44463</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -691,7 +1096,7 @@
         <v>44468</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -714,7 +1119,7 @@
         <v>44407</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -737,7 +1142,7 @@
         <v>44220</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -760,7 +1165,7 @@
         <v>44301</v>
       </c>
       <c r="G11" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -777,13 +1182,13 @@
         <v>5</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="2">
-        <v>44296</v>
+        <v>44262</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -800,13 +1205,13 @@
         <v>5</v>
       </c>
       <c r="E13">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F13" s="2">
-        <v>44195</v>
+        <v>44283</v>
       </c>
       <c r="G13" t="s">
-        <v>37</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -826,10 +1231,10 @@
         <v>0</v>
       </c>
       <c r="F14" s="2">
-        <v>44419</v>
+        <v>44280</v>
       </c>
       <c r="G14" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -849,10 +1254,10 @@
         <v>0</v>
       </c>
       <c r="F15" s="2">
-        <v>44198</v>
+        <v>44347</v>
       </c>
       <c r="G15" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -875,7 +1280,7 @@
         <v>44268</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -892,13 +1297,13 @@
         <v>5</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="2">
-        <v>44256</v>
+        <v>44246</v>
       </c>
       <c r="G17" t="s">
-        <v>40</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -918,10 +1323,10 @@
         <v>0</v>
       </c>
       <c r="F18" s="2">
-        <v>44258</v>
+        <v>44498</v>
       </c>
       <c r="G18" t="s">
-        <v>41</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -941,10 +1346,1666 @@
         <v>0</v>
       </c>
       <c r="F19" s="2">
-        <v>44213</v>
+        <v>44499</v>
       </c>
       <c r="G19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>44391</v>
+      </c>
+      <c r="G20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>44411</v>
+      </c>
+      <c r="G21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <v>44477</v>
+      </c>
+      <c r="G22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>44424</v>
+      </c>
+      <c r="G23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>44368</v>
+      </c>
+      <c r="G24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>44320</v>
+      </c>
+      <c r="G25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>44503</v>
+      </c>
+      <c r="G26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>44507</v>
+      </c>
+      <c r="G27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>44331</v>
+      </c>
+      <c r="G28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>44287</v>
+      </c>
+      <c r="G29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <v>44388</v>
+      </c>
+      <c r="G30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>44297</v>
+      </c>
+      <c r="G31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <v>44316</v>
+      </c>
+      <c r="G32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>44303</v>
+      </c>
+      <c r="G33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <v>44452</v>
+      </c>
+      <c r="G34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>44327</v>
+      </c>
+      <c r="G35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" t="s">
         <v>42</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2">
+        <v>44276</v>
+      </c>
+      <c r="G36" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2">
+        <v>44386</v>
+      </c>
+      <c r="G37" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2">
+        <v>44417</v>
+      </c>
+      <c r="G38" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39">
+        <v>5</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2">
+        <v>44366</v>
+      </c>
+      <c r="G39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <v>5</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40" s="2">
+        <v>44393</v>
+      </c>
+      <c r="G40" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+      <c r="D41">
+        <v>5</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" s="2">
+        <v>44507</v>
+      </c>
+      <c r="G41" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42">
+        <v>5</v>
+      </c>
+      <c r="D42">
+        <v>5</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" s="2">
+        <v>44430</v>
+      </c>
+      <c r="G42" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="D43">
+        <v>5</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43" s="2">
+        <v>44400</v>
+      </c>
+      <c r="G43" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44">
+        <v>5</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44" s="2">
+        <v>44284</v>
+      </c>
+      <c r="G44" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45">
+        <v>5</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45" s="2">
+        <v>44432</v>
+      </c>
+      <c r="G45" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
+      </c>
+      <c r="D46">
+        <v>5</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" s="2">
+        <v>44250</v>
+      </c>
+      <c r="G46" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>5</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" s="2">
+        <v>44366</v>
+      </c>
+      <c r="G47" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48">
+        <v>5</v>
+      </c>
+      <c r="D48">
+        <v>5</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48" s="2">
+        <v>44470</v>
+      </c>
+      <c r="G48" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+      <c r="D49">
+        <v>5</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49" s="2">
+        <v>44283</v>
+      </c>
+      <c r="G49" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50">
+        <v>5</v>
+      </c>
+      <c r="D50">
+        <v>5</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50" s="2">
+        <v>44255</v>
+      </c>
+      <c r="G50" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51">
+        <v>5</v>
+      </c>
+      <c r="D51">
+        <v>5</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" s="2">
+        <v>44292</v>
+      </c>
+      <c r="G51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52">
+        <v>6</v>
+      </c>
+      <c r="D52">
+        <v>5</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52" s="2">
+        <v>44399</v>
+      </c>
+      <c r="G52" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53">
+        <v>6</v>
+      </c>
+      <c r="D53">
+        <v>5</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" s="2">
+        <v>44500</v>
+      </c>
+      <c r="G53" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54">
+        <v>6</v>
+      </c>
+      <c r="D54">
+        <v>5</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54" s="2">
+        <v>44259</v>
+      </c>
+      <c r="G54" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55">
+        <v>6</v>
+      </c>
+      <c r="D55">
+        <v>5</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55" s="2">
+        <v>44267</v>
+      </c>
+      <c r="G55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" t="s">
+        <v>60</v>
+      </c>
+      <c r="C56">
+        <v>6</v>
+      </c>
+      <c r="D56">
+        <v>5</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56" s="2">
+        <v>44293</v>
+      </c>
+      <c r="G56" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57">
+        <v>6</v>
+      </c>
+      <c r="D57">
+        <v>5</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57" s="2">
+        <v>44389</v>
+      </c>
+      <c r="G57" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58">
+        <v>6</v>
+      </c>
+      <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58" s="2">
+        <v>44263</v>
+      </c>
+      <c r="G58" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" t="s">
+        <v>63</v>
+      </c>
+      <c r="C59">
+        <v>6</v>
+      </c>
+      <c r="D59">
+        <v>5</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59" s="2">
+        <v>44351</v>
+      </c>
+      <c r="G59" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60">
+        <v>6</v>
+      </c>
+      <c r="D60">
+        <v>5</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60" s="2">
+        <v>44268</v>
+      </c>
+      <c r="G60" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61">
+        <v>6</v>
+      </c>
+      <c r="D61">
+        <v>5</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61" s="2">
+        <v>44332</v>
+      </c>
+      <c r="G61" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62">
+        <v>7</v>
+      </c>
+      <c r="D62">
+        <v>5</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62" s="2">
+        <v>44270</v>
+      </c>
+      <c r="G62" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63">
+        <v>7</v>
+      </c>
+      <c r="D63">
+        <v>5</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63" s="2">
+        <v>44376</v>
+      </c>
+      <c r="G63" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" t="s">
+        <v>68</v>
+      </c>
+      <c r="C64">
+        <v>7</v>
+      </c>
+      <c r="D64">
+        <v>5</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64" s="2">
+        <v>44448</v>
+      </c>
+      <c r="G64" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" t="s">
+        <v>69</v>
+      </c>
+      <c r="C65">
+        <v>7</v>
+      </c>
+      <c r="D65">
+        <v>5</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65" s="2">
+        <v>44424</v>
+      </c>
+      <c r="G65" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66">
+        <v>7</v>
+      </c>
+      <c r="D66">
+        <v>5</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66" s="2">
+        <v>44351</v>
+      </c>
+      <c r="G66" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" t="s">
+        <v>71</v>
+      </c>
+      <c r="C67">
+        <v>7</v>
+      </c>
+      <c r="D67">
+        <v>5</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67" s="2">
+        <v>44356</v>
+      </c>
+      <c r="G67" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>7</v>
+      </c>
+      <c r="B68" t="s">
+        <v>72</v>
+      </c>
+      <c r="C68">
+        <v>7</v>
+      </c>
+      <c r="D68">
+        <v>5</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68" s="2">
+        <v>44451</v>
+      </c>
+      <c r="G68" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>7</v>
+      </c>
+      <c r="B69" t="s">
+        <v>73</v>
+      </c>
+      <c r="C69">
+        <v>7</v>
+      </c>
+      <c r="D69">
+        <v>5</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69" s="2">
+        <v>44417</v>
+      </c>
+      <c r="G69" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" t="s">
+        <v>74</v>
+      </c>
+      <c r="C70">
+        <v>7</v>
+      </c>
+      <c r="D70">
+        <v>5</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70" s="2">
+        <v>44234</v>
+      </c>
+      <c r="G70" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" t="s">
+        <v>7</v>
+      </c>
+      <c r="B71" t="s">
+        <v>75</v>
+      </c>
+      <c r="C71">
+        <v>7</v>
+      </c>
+      <c r="D71">
+        <v>5</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71" s="2">
+        <v>44228</v>
+      </c>
+      <c r="G71" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72" t="s">
+        <v>76</v>
+      </c>
+      <c r="C72">
+        <v>8</v>
+      </c>
+      <c r="D72">
+        <v>5</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72" s="2">
+        <v>44246</v>
+      </c>
+      <c r="G72" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B73" t="s">
+        <v>77</v>
+      </c>
+      <c r="C73">
+        <v>8</v>
+      </c>
+      <c r="D73">
+        <v>5</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73" s="2">
+        <v>44443</v>
+      </c>
+      <c r="G73" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" t="s">
+        <v>78</v>
+      </c>
+      <c r="C74">
+        <v>8</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74" s="2">
+        <v>44201</v>
+      </c>
+      <c r="G74" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
+        <v>7</v>
+      </c>
+      <c r="B75" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75">
+        <v>8</v>
+      </c>
+      <c r="D75">
+        <v>5</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75" s="2">
+        <v>44388</v>
+      </c>
+      <c r="G75" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" t="s">
+        <v>48</v>
+      </c>
+      <c r="C76">
+        <v>8</v>
+      </c>
+      <c r="D76">
+        <v>5</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76" s="2">
+        <v>44453</v>
+      </c>
+      <c r="G76" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" t="s">
+        <v>7</v>
+      </c>
+      <c r="B77" t="s">
+        <v>80</v>
+      </c>
+      <c r="C77">
+        <v>8</v>
+      </c>
+      <c r="D77">
+        <v>5</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77" s="2">
+        <v>44254</v>
+      </c>
+      <c r="G77" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" t="s">
+        <v>7</v>
+      </c>
+      <c r="B78" t="s">
+        <v>81</v>
+      </c>
+      <c r="C78">
+        <v>8</v>
+      </c>
+      <c r="D78">
+        <v>5</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78" s="2">
+        <v>44431</v>
+      </c>
+      <c r="G78" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" t="s">
+        <v>7</v>
+      </c>
+      <c r="B79" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79">
+        <v>8</v>
+      </c>
+      <c r="D79">
+        <v>5</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79" s="2">
+        <v>44437</v>
+      </c>
+      <c r="G79" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" t="s">
+        <v>7</v>
+      </c>
+      <c r="B80" t="s">
+        <v>83</v>
+      </c>
+      <c r="C80">
+        <v>8</v>
+      </c>
+      <c r="D80">
+        <v>5</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80" s="2">
+        <v>44258</v>
+      </c>
+      <c r="G80" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" t="s">
+        <v>7</v>
+      </c>
+      <c r="B81" t="s">
+        <v>84</v>
+      </c>
+      <c r="C81">
+        <v>8</v>
+      </c>
+      <c r="D81">
+        <v>5</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81" s="2">
+        <v>44356</v>
+      </c>
+      <c r="G81" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" t="s">
+        <v>7</v>
+      </c>
+      <c r="B82" t="s">
+        <v>48</v>
+      </c>
+      <c r="C82">
+        <v>9</v>
+      </c>
+      <c r="D82">
+        <v>5</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82" s="2">
+        <v>44436</v>
+      </c>
+      <c r="G82" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" t="s">
+        <v>7</v>
+      </c>
+      <c r="B83" t="s">
+        <v>85</v>
+      </c>
+      <c r="C83">
+        <v>9</v>
+      </c>
+      <c r="D83">
+        <v>5</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83" s="2">
+        <v>44400</v>
+      </c>
+      <c r="G83" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
+        <v>7</v>
+      </c>
+      <c r="B84" t="s">
+        <v>25</v>
+      </c>
+      <c r="C84">
+        <v>9</v>
+      </c>
+      <c r="D84">
+        <v>5</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84" s="2">
+        <v>44294</v>
+      </c>
+      <c r="G84" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" t="s">
+        <v>7</v>
+      </c>
+      <c r="B85" t="s">
+        <v>86</v>
+      </c>
+      <c r="C85">
+        <v>9</v>
+      </c>
+      <c r="D85">
+        <v>5</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85" s="2">
+        <v>44444</v>
+      </c>
+      <c r="G85" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" t="s">
+        <v>7</v>
+      </c>
+      <c r="B86" t="s">
+        <v>87</v>
+      </c>
+      <c r="C86">
+        <v>9</v>
+      </c>
+      <c r="D86">
+        <v>5</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86" s="2">
+        <v>44415</v>
+      </c>
+      <c r="G86" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" t="s">
+        <v>7</v>
+      </c>
+      <c r="B87" t="s">
+        <v>88</v>
+      </c>
+      <c r="C87">
+        <v>9</v>
+      </c>
+      <c r="D87">
+        <v>5</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87" s="2">
+        <v>44241</v>
+      </c>
+      <c r="G87" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" t="s">
+        <v>7</v>
+      </c>
+      <c r="B88" t="s">
+        <v>89</v>
+      </c>
+      <c r="C88">
+        <v>9</v>
+      </c>
+      <c r="D88">
+        <v>5</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88" s="2">
+        <v>44262</v>
+      </c>
+      <c r="G88" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" t="s">
+        <v>7</v>
+      </c>
+      <c r="B89" t="s">
+        <v>90</v>
+      </c>
+      <c r="C89">
+        <v>9</v>
+      </c>
+      <c r="D89">
+        <v>5</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89" s="2">
+        <v>44245</v>
+      </c>
+      <c r="G89" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" t="s">
+        <v>7</v>
+      </c>
+      <c r="B90" t="s">
+        <v>91</v>
+      </c>
+      <c r="C90">
+        <v>9</v>
+      </c>
+      <c r="D90">
+        <v>5</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90" s="2">
+        <v>44369</v>
+      </c>
+      <c r="G90" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" t="s">
+        <v>7</v>
+      </c>
+      <c r="B91" t="s">
+        <v>92</v>
+      </c>
+      <c r="C91">
+        <v>9</v>
+      </c>
+      <c r="D91">
+        <v>5</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91" s="2">
+        <v>44489</v>
+      </c>
+      <c r="G91" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The review scraper can now take the output spreadsheet from the url scraper as an input.
</commit_message>
<xml_diff>
--- a/product_reviews.xlsx
+++ b/product_reviews.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="315">
   <si>
     <t>product</t>
   </si>
@@ -37,7 +37,13 @@
     <t>body</t>
   </si>
   <si>
-    <t>LEGO 42123 Technic McLaren Senna GTR Racing Sports Collectable Model Car, Vehicle Toy Construction Set, Idea</t>
+    <t>LEGO 42123 Technic McLaren Senna GTR Racing Sports Collectable Model Car, Vehicle Construction Set, Toy Gift Idea</t>
+  </si>
+  <si>
+    <t>LEGO 76196 Marvel The Avengers Advent Calendar 2021 Buildable Toys with Spider-Man and Iron Man for Kids Aged 7 Idea</t>
+  </si>
+  <si>
+    <t>LEGO 41679 Friends Forest House Toy, Treehouse Adventure Set with Mia Mini Doll and Kayak Boat Model</t>
   </si>
   <si>
     <t>You'll be happy to build this</t>
@@ -49,6 +55,9 @@
     <t>Brilliant model</t>
   </si>
   <si>
+    <t>Brilliant build quality for my 7yo</t>
+  </si>
+  <si>
     <t>Good beginner set, now im hooked</t>
   </si>
   <si>
@@ -58,9 +67,6 @@
     <t>Great model, but a little fiddly.</t>
   </si>
   <si>
-    <t>Brilliant build quality for my 7yo</t>
-  </si>
-  <si>
     <t>Best value for money Lego Technic car available</t>
   </si>
   <si>
@@ -157,6 +163,9 @@
     <t>Senna car</t>
   </si>
   <si>
+    <t>Great price, genuine product</t>
+  </si>
+  <si>
     <t>Technic McLaren</t>
   </si>
   <si>
@@ -241,6 +250,9 @@
     <t>McLaren Senna GTR</t>
   </si>
   <si>
+    <t>Xmas Lego</t>
+  </si>
+  <si>
     <t>Great to build always enjoy Lego.</t>
   </si>
   <si>
@@ -289,12 +301,195 @@
     <t>Make sure you get the right component as many are very simular</t>
   </si>
   <si>
-    <t>Fun to Build</t>
+    <t>Get it now before the inevitable stock shortage in November!</t>
+  </si>
+  <si>
+    <t>One of the best calendars last few years</t>
+  </si>
+  <si>
+    <t>Fast delivery</t>
+  </si>
+  <si>
+    <t>Bought for Grandson</t>
+  </si>
+  <si>
+    <t>Awesome set</t>
+  </si>
+  <si>
+    <t>Damaged and repaired with tape</t>
+  </si>
+  <si>
+    <t>Bought as a present from a wish list. Have to assume they will be happy with what they wished for.</t>
+  </si>
+  <si>
+    <t>Perfect</t>
+  </si>
+  <si>
+    <t>Very quick and great value</t>
+  </si>
+  <si>
+    <t>Thanks</t>
+  </si>
+  <si>
+    <t>Worth every penny</t>
+  </si>
+  <si>
+    <t>Very good</t>
+  </si>
+  <si>
+    <t>Covered in Coffee</t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>Amazing</t>
+  </si>
+  <si>
+    <t>All looks perfect and in one piece very happy indeed</t>
+  </si>
+  <si>
+    <t>What you would expect</t>
+  </si>
+  <si>
+    <t>Love it 😍</t>
+  </si>
+  <si>
+    <t>Super cute build</t>
+  </si>
+  <si>
+    <t>Super set for a very good price</t>
+  </si>
+  <si>
+    <t>keeps the kids happy and amused</t>
+  </si>
+  <si>
+    <t>Genuine Lego- lots of fun</t>
+  </si>
+  <si>
+    <t>EGO 41679 Friends Forest House</t>
+  </si>
+  <si>
+    <t>Christmas</t>
+  </si>
+  <si>
+    <t>Great set!</t>
+  </si>
+  <si>
+    <t>Little Julia will love it. .. xx</t>
+  </si>
+  <si>
+    <t>Xmas gift grandaughter</t>
+  </si>
+  <si>
+    <t>Purchased as a present</t>
+  </si>
+  <si>
+    <t>Awesome</t>
+  </si>
+  <si>
+    <t>My granddaughter loved this Friends Lego that l bought for her</t>
+  </si>
+  <si>
+    <t>REALLY good</t>
+  </si>
+  <si>
+    <t>Good present for grandaughter</t>
+  </si>
+  <si>
+    <t>Great set</t>
+  </si>
+  <si>
+    <t>Very good product kept my 6 yr old busy</t>
+  </si>
+  <si>
+    <t>Lovely Tree house our little boy especially liked the loo</t>
+  </si>
+  <si>
+    <t>Good Value Set</t>
+  </si>
+  <si>
+    <t>Makes you want to go camping</t>
+  </si>
+  <si>
+    <t>Lego Friends 41679: Forest House</t>
+  </si>
+  <si>
+    <t>Another great LEGO Friends set - we particularly like the kayaking aspect!</t>
+  </si>
+  <si>
+    <t>An excellent toy</t>
+  </si>
+  <si>
+    <t>Cute set, fun build, lots of play</t>
+  </si>
+  <si>
+    <t>Great set - features and contents</t>
+  </si>
+  <si>
+    <t>Its Lego. Its Great!</t>
+  </si>
+  <si>
+    <t>Lego Friends Forest House Playset</t>
+  </si>
+  <si>
+    <t>Very cute set</t>
+  </si>
+  <si>
+    <t>Excellent play value.</t>
+  </si>
+  <si>
+    <t>A delightful toy for a child</t>
+  </si>
+  <si>
+    <t>Great Lego Friends set</t>
+  </si>
+  <si>
+    <t>Great value set</t>
+  </si>
+  <si>
+    <t>Wonderful set</t>
+  </si>
+  <si>
+    <t>Fun and easy to assemble</t>
+  </si>
+  <si>
+    <t>Lovely little tree house</t>
+  </si>
+  <si>
+    <t>Perfect Xmas present!</t>
+  </si>
+  <si>
+    <t>LEGO 41679 Friends Forest House Toy, Treehouse Adventure Set with Mia Mini Doll and Kayak</t>
+  </si>
+  <si>
+    <t>Cute set</t>
+  </si>
+  <si>
+    <t>Lovely set</t>
+  </si>
+  <si>
+    <t>a huge and detailed fun set</t>
+  </si>
+  <si>
+    <t>Cute little set</t>
+  </si>
+  <si>
+    <t>Great Set</t>
+  </si>
+  <si>
+    <t>Great Wee Tree house Toy</t>
   </si>
   <si>
     <t>Great</t>
   </si>
   <si>
+    <t>happy child</t>
+  </si>
+  <si>
+    <t>Bargain</t>
+  </si>
+  <si>
     <t>A very nice set to make, numbered bags are also a really big help, for the price it's a really good set</t>
   </si>
   <si>
@@ -304,6 +499,9 @@
     <t>Thoroughly enjoyed making this car. It is sufficiently demanding to make it a worthwhile task. I went wrong a couple of times, which meant a bit of dismantling. However, got there in the end and it makes a great display model. Difficulty is keeping young probing fingers away. Highly recommended and a saving on price at Amazon.</t>
   </si>
   <si>
+    <t>This was bought for a birthday present from my 7yo son to his Daddy for them to do together, but my son ended up doing it all himself - he absolutely loved it! He loves Lego Technics builds and did this one in 3/4 sittings, even getting up early before school to do it, he enjoyed it so much. Some technics kits are very expensive so this was great value for money and my son loved doing it and now plays with the finished product.</t>
+  </si>
+  <si>
     <t>My first technic set and my first lego set since i was 14 or so (31 now) and enjoyed this throughout.A not too complex set but at the same time still clever. Took around 3 hours to do the whole thing and i would say only one but frustrated me which involved the piece 6282140 (Pin with Friction Ridges Lengthwise and Pin Hole) as its hard to push them into a hole whilst they also spin around which was for the windscreen frame near the end.Overall i enjoyed this and am hooked on building again. Only complaint is lots of stickers which im not great at but tweezers helped.</t>
   </si>
   <si>
@@ -313,9 +511,6 @@
     <t>Lego isn't cheap, but for around £30 this, in my opinion, offers good value for money.A high part count, coupled with decent instructions (although they could be clearer in places) produces a lovely looking finished product.I do get a little annoyed at Lego's propensity for producing new pieces for specific shapes rather than using multiple existing parts to get the same result.  Somehow, it takes away from the challenge I experienced many years ago with the very first technical lego kits.</t>
   </si>
   <si>
-    <t>This was bought for a birthday present from my 7yo son to his Daddy for them to do together, but my son ended up doing it all himself - he absolutely loved it! He loves Lego Technics builds and did this one in 3/4 sittings, even getting up early before school to do it, he enjoyed it so much. Some technics kits are very expensive so this was great value for money and my son loved doing it and now plays with the finished product.</t>
-  </si>
-  <si>
     <t>Pros- Extremely good value for money when you break down how many pieces you get compared to how much the set costs- The stickers that come with the product are unique, and make the finished product look very premium compared to other Lego products- The colour scheme is great.Cons:- It's lego, so compared to other brick products the value for money isn't that high. But you are paying for a superior product.Overall: This makes the product look great as a display piece once it's done, and it's enjoyable to build it with just the right amount of parts.</t>
   </si>
   <si>
@@ -415,6 +610,9 @@
     <t>Some fiddly bits ,youngsters will need help,otherwise,good 🤩</t>
   </si>
   <si>
+    <t>Genuine product, the price was great. It was a gift.</t>
+  </si>
+  <si>
     <t>Bought for 7 year old grandson - he loves it 👍</t>
   </si>
   <si>
@@ -493,6 +691,9 @@
     <t>Thanks 🤩 Excellent design and kept me occupied for several days doing the assembly good fun and very interesting 👍👍</t>
   </si>
   <si>
+    <t>Bought it for xmas present so one exicted big boy for his xmas</t>
+  </si>
+  <si>
     <t>It fits on my Lego car transporter perfectly.</t>
   </si>
   <si>
@@ -544,10 +745,221 @@
     <t>Easy to assemble, and a good price for the size</t>
   </si>
   <si>
-    <t>The Lego set was quite tricky to build but I managed to do it</t>
-  </si>
-  <si>
-    <t>Christmas present sorted</t>
+    <t>Slightly expensive for an advent calendar?? Maybe…but the look on my son’s face when he sees this on December the 1st will be priceless! Mind you, I’m also excited to open this with him!He’s had a Lego advent calendar since he was born, and I’ve had one since before he was born! So it’s great to carry on the tradition, and this Marvel calendar looks set to be one of the best ones we’ve had!Last year I had a slight issue with his Harry Potter Lego Advent calendar whereby he had two of the same items on different days, meaning he didn’t have the ‘main Harry Potter Lego minifig’ he should have had on day one, but after getting in touch with Lego they sent me out the replacement minifig quick as a jif, so he was able to complete his set in time for Christmas Day. I thought it best this time to check that everything was as it should be - and luckily it was - if I were you, I’d check when you get it to avoid any disappointment, it’s easy enough to slip a knife through the sellotape to open up the box and slide out the holders, although be careful to make everything goes back where it came from, as the individual build instructions are obviously on the window interior when you open it up.If you don’t fancy doing that, and are willing to gamble, there shouldn’t be an issue really I think I was just unlucky last year, but, if there is an issue I’m sure Lego with their great customer service will put it right quick as a jif!!Can’t really give a proper review of the set until 24th December as that’s when it will be fully realised, but I’ll update my review then - although, it will be too late for anyone else to get one as Lego Advent calendars tend to sell out Mid November if not earlier, so the best advice I can give you is to get one sooner rather than later to avoid disappointment, as this set looks set to be a belter!! I mean, Iron man in a Christmas Jumper, Spider-Man drinking hot chocolate and Thor in a woolly scarf…what’s not to love!!Get one before they sell out!Thanks for reading - if you found this helpful, please let me know by clicking below. 😀</t>
+  </si>
+  <si>
+    <t>Plenty of items for each day unlike other lego calendars over the last few years which have been a bit poor. Very good value as well.</t>
+  </si>
+  <si>
+    <t>Delivery was prompt, and the price was good as they hadn't stuck an extra £5 on like most sellers who aren't a major well known shop. We normally buy this sort of thing direct from The Lego Shop, but they were constantly sold out, making the price of this one even better.</t>
+  </si>
+  <si>
+    <t>Not opened yet as it’s not December but going on previous Lego products it will be great</t>
+  </si>
+  <si>
+    <t>My grandson is marvel fan so will enjoy opening them over 24 day to Christmas. Good buy</t>
+  </si>
+  <si>
+    <t>The first ever Lego Avengers Advent Calendar. There have been rumours about these going out of stock due to supply issues. Super happy to get one, thanks. Can't wait for Christmas!</t>
+  </si>
+  <si>
+    <t>Funny if wasn't true. Package game. If it's clear in the photo's, they've taoed up the ripped bits, stuck it in the post and sent it to us.I don't normally write reviews, but the audaciousness of this particular company os worth warning others about. Most assuredly, AVOID!</t>
+  </si>
+  <si>
+    <t>Bought as a present. Won't be opened and assembled till December as it is an advent calendar. Assume as there are so few parts it will be easy to assemble. Was the same price on other sites.</t>
+  </si>
+  <si>
+    <t>Good value my grandson will love it.</t>
+  </si>
+  <si>
+    <t>Can't wait till my grandson opens it</t>
+  </si>
+  <si>
+    <t>Great item</t>
+  </si>
+  <si>
+    <t>Buy these every year and worth every penny if you are a Lego fan</t>
+  </si>
+  <si>
+    <t>Very good legooo</t>
+  </si>
+  <si>
+    <t>Arrived and the box is covered in Coffee stains and sticky. When I opened it to get to where the doors are it all ripped so cannot be used as an Advent Calendar.</t>
+  </si>
+  <si>
+    <t>Arrived early but nit opened yet, although gave biught before and was very happy.</t>
+  </si>
+  <si>
+    <t>My grandson will be over the moon</t>
+  </si>
+  <si>
+    <t>I would recommend. The minifigures are very detailed. Mainly brought for all the infinity stones and gauntlet</t>
+  </si>
+  <si>
+    <t>Looks good will see what's its like come the 1st dec</t>
+  </si>
+  <si>
+    <t>It's exactly that you expect it to be, it's lego</t>
+  </si>
+  <si>
+    <t>Perfect advent calendar for any Lego/Marvel fan. Plenty of mini figures included and lots of other bits to build and accessories too 👍</t>
+  </si>
+  <si>
+    <t>Was on the fence about getting this set, but saw it was on offer on Amazon and decided to purchase. So glad I did as it is so pretty. Makes a lovely display piece, but the play value is great. Love the canoe and the barbecue.</t>
+  </si>
+  <si>
+    <t>It was a birthday gift for our great grandaughter, she was eager to start making it as soon as she opened it. She went to Legoland and loved it, had a brilliant time.</t>
+  </si>
+  <si>
+    <t>I bought this as part of a Christmas present so we have not built it yet, but it looks amazing and was so reasonably priced compared to other shops. I'd definitely recommend it.</t>
+  </si>
+  <si>
+    <t>keeps the kids amused for ages, very easy to follow instructions and looks great when fully built up.will keep any lego fan happy!</t>
+  </si>
+  <si>
+    <t>My girl loves this. She is 5 years old. The instructions are simple to follow. She enjoyed the little pieces and figures. Has been playing with it for many days in the row. Great buy!</t>
+  </si>
+  <si>
+    <t>Got this for granddaughter’s birthday, was so nice to see her happy face when she opened</t>
+  </si>
+  <si>
+    <t>Bought for my granddaughters birthday she is delighted therefore I’m a happy grandma</t>
+  </si>
+  <si>
+    <t>Brought for Christmas  looks good well packaged very happy with purchase</t>
+  </si>
+  <si>
+    <t>My 6 year old daughter absolutely loves this set and put a lot of it together by herself.</t>
+  </si>
+  <si>
+    <t>Looks great, very tempted myself toOpen up the box &amp; having a build !!</t>
+  </si>
+  <si>
+    <t>Great value style and suitable age group and delivery quick</t>
+  </si>
+  <si>
+    <t>Great lego set.  Cheaper than in store.</t>
+  </si>
+  <si>
+    <t>I believe my granddaughter loved it</t>
+  </si>
+  <si>
+    <t>Great Lego gift!!</t>
+  </si>
+  <si>
+    <t>Amazing product</t>
+  </si>
+  <si>
+    <t>A present for my 6 year old granddaughter. Loves it.</t>
+  </si>
+  <si>
+    <t>Really good</t>
+  </si>
+  <si>
+    <t>As described. Child couldn’t be happier</t>
+  </si>
+  <si>
+    <t>really good products</t>
+  </si>
+  <si>
+    <t>Grandaughter really enjoyed this set</t>
+  </si>
+  <si>
+    <t>Lego, say no more.</t>
+  </si>
+  <si>
+    <t>My daughter was very happy with this set and it was great value too, cheaper than other retailers</t>
+  </si>
+  <si>
+    <t>Good value for money, kept 6 yr old entertained for ages.</t>
+  </si>
+  <si>
+    <t>This set is for our little boy who isn't old enough at 3 and a half to make this set, but has enjoyed playing with it immensely. He especially likes the toilet in the tree trunk and everyone and their dog from our lego collection has been for a wee wee since we got this. The build was straightforward and rewarding with the toilet and BBQ being my favourite bits. The Canoe is a nice addition as we didn't have one beforehand, I also like the fact that the roof hinges open to get access to the beds in the roof. There are three mini figures and a racoon to play with as well as some hotdogs for the bbq.A decent amount of lego for £25 with the build being a bit more 3D and playable from all angles than some other lego friends sets. Very happy to recommend!</t>
+  </si>
+  <si>
+    <t>Great value set. A 2 floor summer treehouse - inside there’s a sleeping area, toilet and entrance complete with a basin. Outside is a patio with a sofa and barbecue. A separate toy river scene and kayak model is included. Comes with 2 mini-dolls, a LEGO Friends Ava micro-doll and a raccoon toy. Accessories include ketchup and mustard bottles, a hotdog, camera, kayak, life vest and paddle.The LEGO forest dollhouse measures over 7 in. (18 cm) high, 7 in. (19 cm) wide and 4 in. (11 cm) deep.My niece loves lego and was able to assemble this with no help.Recommended and good value at RRP of £24.99</t>
+  </si>
+  <si>
+    <t>You really can’t go wrong with lego and this lego friends is no different.I ordered this for my 6 year old nephew to play with his best friend and the two of them loved it.This is a bright and colourful tree house with some outdoor accessories (canoe for example), which remind me of camping- even down to the little hotdog.What I really like about these playsets is once you’ve made the items out of lego, you can turn them in to a playset and engage in pretend play.  I love how this encourages imaginative play for hours on end.  It helps having the little figures provided so you can ‘pretend’ they are off having adventures.Attention to detail on this is brilliant, making it a great overall toy.Lego appears sturdy and well made; perfectly able to be broken up and made again many times.Priced at around £20 feels really reasonable for lego.Overall we’ve been happy with this and more than happy to recommend.</t>
+  </si>
+  <si>
+    <t>This is one of the smaller new forest theme sets from Friends but whilst its one of the smallest its really good value for money as comes with three figures and it has lots of play value.The set includes two minifigures Mia and Ann and also one of the new minidolls Ava.  There is also a little Raccoon.The set has 326 parts along with a few spare pieces and does have stickers that need to be applied (we aren't sticker fans as they can be a pain to get straight).Along with the forest house there is a kayak and little forest area to build and my Daughter has attached this to one of her blue base plates in her room to make a lake.The house is little but manages to pack in the essentials such as a toilet, sleeping area (with opening roof to look at the stars), sink and an outdoor seating area and grill.</t>
+  </si>
+  <si>
+    <t>The LEGO Friends range is always a particularly feminine line, which was initially disappointing in its focus on more stereotypical interests for girls but which has definitely improved over time. This Treehouse Adventure Set, like all the LEGO Friends sets, might have lots of pink and purple, with expressive characters that don't fit the traditional LEGO person style, but the theme of the set is of camping out in a treehouse and going on an adventurous kayaking expedition, which my ten-year-old daughter loved to build and play with afterwards.There's something very fragmented about the LEGO Friends sets - they always seem to come with lots of little accessories, flowers, animals and pieces, so that rather than creating a single diorama or base, you end up with lots of disconnected parts that can be played with together but are easily lost. It makes the sets easy to play with, which my daughter enjoys, though more of a pain for me to store, and consequently I don't feel like they're as easy to take apart and rebuild at a later date as more conventional LEGO sets.It's fair to say that LEGO Friends really doesn't lend itself to imaginative building - I can't see many children buying this set and then taking the pieces apart to stretch their imaginations with their own builds. But for a directed set of instructions for a younger child, with a very cool outcome, this is a fantastic set, with individually numbered bags, easy to follow instructions and nothing so elaborate that they'd need much help from an adult.</t>
+  </si>
+  <si>
+    <t>These sets are excellent, there is so much attention to detail, there are so many tiny parts that are entertaining to adults, not to mention girls and boys alike, that it is definitely not an iddue that there is someone wearing a skirt - these sets are not sexist.  This is another excellent gift idea from Lego. Lego sets ALWAYS have some extremely sweet touches to them - some elements of surprise, something that makes them just that little bit dearer than an ordinary building set, something more memorable and somehow more personalised.  And, luckily, you cannot always guess what that element will be from the pictures or the box, and I do think that unveiling it is not quite fair, you need to have that experience yourself to enjoy it more. There are always some tiny bits that are transparent and look like tiny gems, there are objects of different texture and elasticity/flexibility, there are some compartments and so on.  And every time your child builds the thing up you can proudly display it for some time. AND! They can play with it. The thing is always sufficient enough to allow that.  Another great set, another happy constructing time, another tiny achievement.</t>
+  </si>
+  <si>
+    <t>This is such a fun set from the Lego Friends set, perfect to start your collection or add to it! Aimed at children aged 6+ I feel this set is well suited to the younger Lego builder, it’s fairly simple but has interesting sections to still challenge, for example building some of the smaller details in the interior of the cabin. There are three figures and a tiny cute raccoon which my kids loved! Although I have to say their favourite part has to be the tiny toilet area, they thought this was hilarious and love creating stories where the characters have to rush to the loo whilst out in the forest, so funny! There’s a lovely amount of accessories from tiny hot dogs to the kayak with life vest so much for the budding Lego fans to get their hands on to creative imaginative play scenarios for their Friends characters. The set is great value, so much to build and play with and would make for a great gift, or maybe even as a reward for a reward chart!</t>
+  </si>
+  <si>
+    <t>This is value for  money. They are enough pieces here for variety of play and the joy of building. Compared to non-Lego toys in this price range - this is a real winner. No batteries needed! Durability guaranteed - the pieces are almost indestructible.Easy to follow diagrams for building (and encourage the youngster to have a go - mine is just about moving on from Duplo so understands but sometimes finds the small pieces tricky to handle).I recommend getting the inexpensive 41677 Forest Waterfall with this set to increase the scenery. Because it's Lego, other - non-Friends - sets can be introduced to make up a community.My only niggle - as one collects from the series the child ends up with multiples of the same character seeing as each set comes with some.</t>
+  </si>
+  <si>
+    <t>In my view this Lego Friends Forest House set is a long way from the Lego I was bought up with. In my day (I'm going back to the 1960s of course) all you got in a Lego set was a variety of square and rectangular bricks. this set contains so much more, things like trees, people, pets and even movable parts. Its barely recognisable as a Lego set to my older eyes. What both the old Lego and the modern day Lego both have in common though is that the high quality of the parts and the attraction it has to children. Our niece was so thrilled when we gave her this set. its engrossed her for hours each day for over a week now. great for her imagination, creative development and keeping her entertained on rainy summer days.</t>
+  </si>
+  <si>
+    <t>The playset requires minimal building as a lot of pieces come prebuilt and just clip together. There are good instructions with clear pictures to follow to assemble the play set. This set would fit together with other sets in the same range to give more playability. The set comes with many accessories and details plus two mini figures and a tiny doll figure. The mini figures feature removable hair so that they can wear a helmet, hands that can clip onto accessories and bendable bodies so that they can sit. The house has clip together furnishings and a roof that raises so the figures can stand upright in the roof/bedroom area. The kayak accessory comes with a separate stand and scenery. A good value for money playset.</t>
+  </si>
+  <si>
+    <t>This is a brilliant Treehouse set from Lego Friends, the younger version of Lego. My daughter absolutely loves Lego Friends and likes that the figures are bigger than regular Lego figures and have more detail and are also easier to build with bigger pieces and easier to assemble parts.The Treehouse has some great features, the canoe is very fun and adds to the camping adventure feel. The details are lovely on this and has loads of play value, my daughter has a few of these sets now so she's put them altogether to form a little Lego Friends community, she loves them!Recommended, a nice little set and a fun addition to my daughters collection!</t>
+  </si>
+  <si>
+    <t>This is a really good Lego set.The set takes a little time to assemble, it’s not a 10 minute job and in places some adult help is required, making this an exciting toy to build together and reinforce the importance of team work, as well as chat, develop conflict and conversations skills as well as fine motor skills.When built the set is really pretty and can be played with ( some pieces flew off but they were soon put back on).Being Lego, you know the quality and longevity of the bricks ( we still have some from the 80’s,) and it will, of course, work with other Lego sets you may already have.The Lego ladies are sweet and fairly detailed so you can identify each character.</t>
+  </si>
+  <si>
+    <t>Children love Lego toys - and they also love tree houses.This is a beautiful gift, which I would say is more suitable for the average girl than a boy. It comes with small figures (including a raccoon!) that they can place in a number of different scenarios.Also supplied is a kayak (which no doubt seems pretty bizarre to us in the UK - and along with the raccoon, probably suggests it was originally targeted at the American market) but this all adds to the fun.There’s lots for a child to play with, and the whole thing is very colourful and delightful, but it’s probably not suited to really young children as there are a few pieces that look easy to swallow.</t>
+  </si>
+  <si>
+    <t>I love this Lego set specifically aimed for girls which promotes outdoor and active fun.The treehouse is on 3 floors, with a toilet, bedroom and kitchen area. My niece loved the pop up roof!We have a canoe so you can imagine that after constructing this set she wanted to have a go - all now arranged for next weekend!I think this set is good value at £24.99.Happy to recommend and 5 stars from me.I hope you find my review helpful 😊</t>
+  </si>
+  <si>
+    <t>This is a really fun and vibrant set! It is excellent value for money at the current price of £18.50. There are 326 pieces but it is really simple to build with the comprehensive instructions.It can be used alone or as part of the Friends Forest range. It comes with cute figures and great little accessories. The accessories really have attention to details which stimulate the imagination.I highly recommend this set.</t>
+  </si>
+  <si>
+    <t>Lego will never grow old nor will I tire of it. I fairness, I now buy it for my children as opposed to myself.  This is a lovely treehouse set. It comes complete with a range of accessories and will make for hours of play. My daughter was able to put this together quite easily and by using the simple to follow instructions.  It’s lovely once assembled- reasonably priced too makes for a strong recommendation from me 😀🥰👍</t>
+  </si>
+  <si>
+    <t>Lovely lego addition which is nicely packaged and presented with easy to follow instructions. My youngest has enjoyed building it and was pleasantly straight forward to do and ive noticed she spends more time with this then her other collections keeping her occupied.Theres authentic detail and also clever design for perfect creativity. High quality bits as you’d expect.Excellent value for money overall and we highly recommend it.</t>
+  </si>
+  <si>
+    <t>For the price of this alone being Lego is great and very reasonable, the set is smaller but still lots of fun and great fine motor skill practice for younger children whiile playing with it, theres easy instructions on how to build the house but my kids like to use their imagination and see what else they can build. I'm really happy with it, lego is known for being great quality and this is no exception.</t>
+  </si>
+  <si>
+    <t>It is Lego after all, right? The set is absolutely amazing, quality is second to none, as you would expect from Lego! My little niece was over the Moon and really enjoyed this set. We have sadly lost a couple of bits now, but this has been the most popular set over the ast 6 weeks and has been played with more than I can count! And this is a testament of how engaging it is! Highly recommended!</t>
+  </si>
+  <si>
+    <t>Who's kids don't like Lago. Even as a kid I loved it.This set is very nice and easy to build. Won't take kids long to build it and enjoy it for years to come.Very nice set at a very nice price. Well worth buying.Giving it top marks. My neice will love this set. Gets 5-5 for a top quality set.</t>
+  </si>
+  <si>
+    <t>This is a cute Lego Friends set that includes two adults and one tiny child, who is especially cute.  There is also a little raccoon, which I've not seen before.  The set is a small treehouse with simple facilities inside, and there's also a canoe/kayak which comes with a helmet (very important).</t>
+  </si>
+  <si>
+    <t>This treehouse is lovely! I particularly like the raccoon mini figure! My daughter is a huge fan of the lego freinds program and built this with just a little help at the age of 8. Once complete it’s a lovely sturdy set complete with a kayak and 2 mini figures from the series</t>
+  </si>
+  <si>
+    <t>Friends give the perfect scale play toys for children and once made up stays up for endless play and adventure-Most of the sets can interconnect with all child figures nd build a large play area of activity for hours-the detail is marvelous and is appreciated.</t>
+  </si>
+  <si>
+    <t>The media could not be loaded.
+   Great kit! Definitely supervise your child when they’re building it, if you don’t do it for them ;) as there are many small pieces. Brilliant addition to the LEGO friends sets. Kids will spend hours playing with it.</t>
+  </si>
+  <si>
+    <t>My daughter has always loved doing lego and despite getting to an age where she doesn’t play with the sets loves putting them together still. This is a great price with, as usual, easy to follow instructions.</t>
+  </si>
+  <si>
+    <t>This went over very well for the Summer holidays. Usual Lego quality, and my usual mump about official Lego prices. Worth it, though, for quality and match to other sets.</t>
+  </si>
+  <si>
+    <t>A great set. Seems age appropriate. Would make a great gift.</t>
+  </si>
+  <si>
+    <t>My kids loved this set.</t>
+  </si>
+  <si>
+    <t>This is £29 in morrisons, I paid £16 on here. Bargain.</t>
   </si>
 </sst>
 </file>
@@ -909,7 +1321,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:G163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -943,7 +1355,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -958,7 +1370,7 @@
         <v>44194</v>
       </c>
       <c r="G2" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -966,7 +1378,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -981,7 +1393,7 @@
         <v>44315</v>
       </c>
       <c r="G3" t="s">
-        <v>94</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -989,7 +1401,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1004,7 +1416,7 @@
         <v>44333</v>
       </c>
       <c r="G4" t="s">
-        <v>95</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1012,7 +1424,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1021,13 +1433,13 @@
         <v>5</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="2">
-        <v>44500</v>
+        <v>44468</v>
       </c>
       <c r="G5" t="s">
-        <v>96</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1035,7 +1447,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1044,13 +1456,13 @@
         <v>5</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>44430</v>
+        <v>44500</v>
       </c>
       <c r="G6" t="s">
-        <v>97</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1058,7 +1470,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1067,13 +1479,13 @@
         <v>5</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="2">
-        <v>44463</v>
+        <v>44430</v>
       </c>
       <c r="G7" t="s">
-        <v>98</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1081,7 +1493,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1093,10 +1505,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="2">
-        <v>44468</v>
+        <v>44463</v>
       </c>
       <c r="G8" t="s">
-        <v>99</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1104,7 +1516,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1119,7 +1531,7 @@
         <v>44407</v>
       </c>
       <c r="G9" t="s">
-        <v>100</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1127,7 +1539,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1142,7 +1554,7 @@
         <v>44220</v>
       </c>
       <c r="G10" t="s">
-        <v>101</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1150,7 +1562,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1165,7 +1577,7 @@
         <v>44301</v>
       </c>
       <c r="G11" t="s">
-        <v>102</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1173,7 +1585,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1188,7 +1600,7 @@
         <v>44262</v>
       </c>
       <c r="G12" t="s">
-        <v>103</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1196,7 +1608,7 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1211,7 +1623,7 @@
         <v>44283</v>
       </c>
       <c r="G13" t="s">
-        <v>104</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1219,7 +1631,7 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1234,7 +1646,7 @@
         <v>44280</v>
       </c>
       <c r="G14" t="s">
-        <v>105</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1242,7 +1654,7 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -1257,7 +1669,7 @@
         <v>44347</v>
       </c>
       <c r="G15" t="s">
-        <v>106</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1265,7 +1677,7 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1280,7 +1692,7 @@
         <v>44268</v>
       </c>
       <c r="G16" t="s">
-        <v>107</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1288,7 +1700,7 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -1303,7 +1715,7 @@
         <v>44246</v>
       </c>
       <c r="G17" t="s">
-        <v>108</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1311,7 +1723,7 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -1326,7 +1738,7 @@
         <v>44498</v>
       </c>
       <c r="G18" t="s">
-        <v>109</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1334,7 +1746,7 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1349,7 +1761,7 @@
         <v>44499</v>
       </c>
       <c r="G19" t="s">
-        <v>110</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1357,7 +1769,7 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1372,7 +1784,7 @@
         <v>44391</v>
       </c>
       <c r="G20" t="s">
-        <v>111</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1380,7 +1792,7 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1395,7 +1807,7 @@
         <v>44411</v>
       </c>
       <c r="G21" t="s">
-        <v>112</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1403,7 +1815,7 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -1418,7 +1830,7 @@
         <v>44477</v>
       </c>
       <c r="G22" t="s">
-        <v>113</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1426,7 +1838,7 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -1441,7 +1853,7 @@
         <v>44424</v>
       </c>
       <c r="G23" t="s">
-        <v>114</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1449,7 +1861,7 @@
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -1464,7 +1876,7 @@
         <v>44368</v>
       </c>
       <c r="G24" t="s">
-        <v>115</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1472,7 +1884,7 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -1487,7 +1899,7 @@
         <v>44320</v>
       </c>
       <c r="G25" t="s">
-        <v>116</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1495,7 +1907,7 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -1510,7 +1922,7 @@
         <v>44503</v>
       </c>
       <c r="G26" t="s">
-        <v>117</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1518,7 +1930,7 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -1533,7 +1945,7 @@
         <v>44507</v>
       </c>
       <c r="G27" t="s">
-        <v>118</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1541,7 +1953,7 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -1556,7 +1968,7 @@
         <v>44331</v>
       </c>
       <c r="G28" t="s">
-        <v>119</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1564,7 +1976,7 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -1579,7 +1991,7 @@
         <v>44287</v>
       </c>
       <c r="G29" t="s">
-        <v>120</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1587,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -1602,7 +2014,7 @@
         <v>44388</v>
       </c>
       <c r="G30" t="s">
-        <v>121</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1610,7 +2022,7 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C31">
         <v>3</v>
@@ -1625,7 +2037,7 @@
         <v>44297</v>
       </c>
       <c r="G31" t="s">
-        <v>122</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1633,7 +2045,7 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C32">
         <v>4</v>
@@ -1648,7 +2060,7 @@
         <v>44316</v>
       </c>
       <c r="G32" t="s">
-        <v>123</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1656,7 +2068,7 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C33">
         <v>4</v>
@@ -1671,7 +2083,7 @@
         <v>44303</v>
       </c>
       <c r="G33" t="s">
-        <v>124</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1679,7 +2091,7 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C34">
         <v>4</v>
@@ -1694,7 +2106,7 @@
         <v>44452</v>
       </c>
       <c r="G34" t="s">
-        <v>125</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1702,7 +2114,7 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C35">
         <v>4</v>
@@ -1717,7 +2129,7 @@
         <v>44327</v>
       </c>
       <c r="G35" t="s">
-        <v>126</v>
+        <v>191</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1725,7 +2137,7 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C36">
         <v>4</v>
@@ -1740,7 +2152,7 @@
         <v>44276</v>
       </c>
       <c r="G36" t="s">
-        <v>127</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1748,7 +2160,7 @@
         <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C37">
         <v>4</v>
@@ -1763,7 +2175,7 @@
         <v>44386</v>
       </c>
       <c r="G37" t="s">
-        <v>128</v>
+        <v>193</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1771,7 +2183,7 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C38">
         <v>4</v>
@@ -1786,7 +2198,7 @@
         <v>44417</v>
       </c>
       <c r="G38" t="s">
-        <v>129</v>
+        <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1794,7 +2206,7 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C39">
         <v>4</v>
@@ -1809,7 +2221,7 @@
         <v>44366</v>
       </c>
       <c r="G39" t="s">
-        <v>130</v>
+        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1817,7 +2229,7 @@
         <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C40">
         <v>4</v>
@@ -1832,7 +2244,7 @@
         <v>44393</v>
       </c>
       <c r="G40" t="s">
-        <v>131</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1840,7 +2252,7 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C41">
         <v>4</v>
@@ -1855,7 +2267,7 @@
         <v>44507</v>
       </c>
       <c r="G41" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1863,7 +2275,7 @@
         <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C42">
         <v>5</v>
@@ -1875,10 +2287,10 @@
         <v>0</v>
       </c>
       <c r="F42" s="2">
-        <v>44430</v>
+        <v>44510</v>
       </c>
       <c r="G42" t="s">
-        <v>133</v>
+        <v>198</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1886,7 +2298,7 @@
         <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C43">
         <v>5</v>
@@ -1898,10 +2310,10 @@
         <v>0</v>
       </c>
       <c r="F43" s="2">
-        <v>44400</v>
+        <v>44430</v>
       </c>
       <c r="G43" t="s">
-        <v>134</v>
+        <v>199</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1909,7 +2321,7 @@
         <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C44">
         <v>5</v>
@@ -1921,10 +2333,10 @@
         <v>0</v>
       </c>
       <c r="F44" s="2">
-        <v>44284</v>
+        <v>44400</v>
       </c>
       <c r="G44" t="s">
-        <v>135</v>
+        <v>200</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1932,7 +2344,7 @@
         <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C45">
         <v>5</v>
@@ -1944,10 +2356,10 @@
         <v>0</v>
       </c>
       <c r="F45" s="2">
-        <v>44432</v>
+        <v>44284</v>
       </c>
       <c r="G45" t="s">
-        <v>136</v>
+        <v>201</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1955,7 +2367,7 @@
         <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="C46">
         <v>5</v>
@@ -1967,10 +2379,10 @@
         <v>0</v>
       </c>
       <c r="F46" s="2">
-        <v>44250</v>
+        <v>44432</v>
       </c>
       <c r="G46" t="s">
-        <v>137</v>
+        <v>202</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1978,7 +2390,7 @@
         <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="C47">
         <v>5</v>
@@ -1990,10 +2402,10 @@
         <v>0</v>
       </c>
       <c r="F47" s="2">
-        <v>44366</v>
+        <v>44250</v>
       </c>
       <c r="G47" t="s">
-        <v>138</v>
+        <v>203</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -2001,7 +2413,7 @@
         <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C48">
         <v>5</v>
@@ -2013,10 +2425,10 @@
         <v>0</v>
       </c>
       <c r="F48" s="2">
-        <v>44470</v>
+        <v>44366</v>
       </c>
       <c r="G48" t="s">
-        <v>139</v>
+        <v>204</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -2024,7 +2436,7 @@
         <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C49">
         <v>5</v>
@@ -2036,10 +2448,10 @@
         <v>0</v>
       </c>
       <c r="F49" s="2">
-        <v>44283</v>
+        <v>44470</v>
       </c>
       <c r="G49" t="s">
-        <v>140</v>
+        <v>205</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -2047,7 +2459,7 @@
         <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C50">
         <v>5</v>
@@ -2059,10 +2471,10 @@
         <v>0</v>
       </c>
       <c r="F50" s="2">
-        <v>44255</v>
+        <v>44283</v>
       </c>
       <c r="G50" t="s">
-        <v>141</v>
+        <v>206</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -2070,7 +2482,7 @@
         <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C51">
         <v>5</v>
@@ -2082,10 +2494,10 @@
         <v>0</v>
       </c>
       <c r="F51" s="2">
-        <v>44292</v>
+        <v>44255</v>
       </c>
       <c r="G51" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -2093,7 +2505,7 @@
         <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C52">
         <v>6</v>
@@ -2105,10 +2517,10 @@
         <v>0</v>
       </c>
       <c r="F52" s="2">
-        <v>44399</v>
+        <v>44292</v>
       </c>
       <c r="G52" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2116,7 +2528,7 @@
         <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C53">
         <v>6</v>
@@ -2128,10 +2540,10 @@
         <v>0</v>
       </c>
       <c r="F53" s="2">
-        <v>44500</v>
+        <v>44399</v>
       </c>
       <c r="G53" t="s">
-        <v>142</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -2139,7 +2551,7 @@
         <v>7</v>
       </c>
       <c r="B54" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C54">
         <v>6</v>
@@ -2151,10 +2563,10 @@
         <v>0</v>
       </c>
       <c r="F54" s="2">
-        <v>44259</v>
+        <v>44500</v>
       </c>
       <c r="G54" t="s">
-        <v>143</v>
+        <v>208</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2162,7 +2574,7 @@
         <v>7</v>
       </c>
       <c r="B55" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C55">
         <v>6</v>
@@ -2174,10 +2586,10 @@
         <v>0</v>
       </c>
       <c r="F55" s="2">
-        <v>44267</v>
+        <v>44259</v>
       </c>
       <c r="G55" t="s">
-        <v>59</v>
+        <v>209</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2185,7 +2597,7 @@
         <v>7</v>
       </c>
       <c r="B56" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C56">
         <v>6</v>
@@ -2197,10 +2609,10 @@
         <v>0</v>
       </c>
       <c r="F56" s="2">
-        <v>44293</v>
+        <v>44267</v>
       </c>
       <c r="G56" t="s">
-        <v>144</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2208,7 +2620,7 @@
         <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C57">
         <v>6</v>
@@ -2220,10 +2632,10 @@
         <v>0</v>
       </c>
       <c r="F57" s="2">
-        <v>44389</v>
+        <v>44293</v>
       </c>
       <c r="G57" t="s">
-        <v>145</v>
+        <v>210</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2231,22 +2643,22 @@
         <v>7</v>
       </c>
       <c r="B58" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C58">
         <v>6</v>
       </c>
       <c r="D58">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E58">
         <v>0</v>
       </c>
       <c r="F58" s="2">
-        <v>44263</v>
+        <v>44389</v>
       </c>
       <c r="G58" t="s">
-        <v>146</v>
+        <v>211</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2254,22 +2666,22 @@
         <v>7</v>
       </c>
       <c r="B59" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C59">
         <v>6</v>
       </c>
       <c r="D59">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E59">
         <v>0</v>
       </c>
       <c r="F59" s="2">
-        <v>44351</v>
+        <v>44263</v>
       </c>
       <c r="G59" t="s">
-        <v>147</v>
+        <v>212</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2277,7 +2689,7 @@
         <v>7</v>
       </c>
       <c r="B60" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C60">
         <v>6</v>
@@ -2289,10 +2701,10 @@
         <v>0</v>
       </c>
       <c r="F60" s="2">
-        <v>44268</v>
+        <v>44351</v>
       </c>
       <c r="G60" t="s">
-        <v>148</v>
+        <v>213</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2300,7 +2712,7 @@
         <v>7</v>
       </c>
       <c r="B61" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C61">
         <v>6</v>
@@ -2312,10 +2724,10 @@
         <v>0</v>
       </c>
       <c r="F61" s="2">
-        <v>44332</v>
+        <v>44268</v>
       </c>
       <c r="G61" t="s">
-        <v>149</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2323,7 +2735,7 @@
         <v>7</v>
       </c>
       <c r="B62" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C62">
         <v>7</v>
@@ -2335,10 +2747,10 @@
         <v>0</v>
       </c>
       <c r="F62" s="2">
-        <v>44270</v>
+        <v>44332</v>
       </c>
       <c r="G62" t="s">
-        <v>150</v>
+        <v>215</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2346,7 +2758,7 @@
         <v>7</v>
       </c>
       <c r="B63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C63">
         <v>7</v>
@@ -2358,10 +2770,10 @@
         <v>0</v>
       </c>
       <c r="F63" s="2">
-        <v>44376</v>
+        <v>44270</v>
       </c>
       <c r="G63" t="s">
-        <v>151</v>
+        <v>216</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2369,7 +2781,7 @@
         <v>7</v>
       </c>
       <c r="B64" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C64">
         <v>7</v>
@@ -2381,10 +2793,10 @@
         <v>0</v>
       </c>
       <c r="F64" s="2">
-        <v>44448</v>
+        <v>44376</v>
       </c>
       <c r="G64" t="s">
-        <v>152</v>
+        <v>217</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -2392,7 +2804,7 @@
         <v>7</v>
       </c>
       <c r="B65" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C65">
         <v>7</v>
@@ -2404,10 +2816,10 @@
         <v>0</v>
       </c>
       <c r="F65" s="2">
-        <v>44424</v>
+        <v>44448</v>
       </c>
       <c r="G65" t="s">
-        <v>153</v>
+        <v>218</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -2415,7 +2827,7 @@
         <v>7</v>
       </c>
       <c r="B66" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C66">
         <v>7</v>
@@ -2427,10 +2839,10 @@
         <v>0</v>
       </c>
       <c r="F66" s="2">
-        <v>44351</v>
+        <v>44424</v>
       </c>
       <c r="G66" t="s">
-        <v>154</v>
+        <v>219</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -2438,7 +2850,7 @@
         <v>7</v>
       </c>
       <c r="B67" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C67">
         <v>7</v>
@@ -2450,10 +2862,10 @@
         <v>0</v>
       </c>
       <c r="F67" s="2">
-        <v>44356</v>
+        <v>44351</v>
       </c>
       <c r="G67" t="s">
-        <v>155</v>
+        <v>220</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -2461,7 +2873,7 @@
         <v>7</v>
       </c>
       <c r="B68" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C68">
         <v>7</v>
@@ -2473,10 +2885,10 @@
         <v>0</v>
       </c>
       <c r="F68" s="2">
-        <v>44451</v>
+        <v>44356</v>
       </c>
       <c r="G68" t="s">
-        <v>156</v>
+        <v>221</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -2484,7 +2896,7 @@
         <v>7</v>
       </c>
       <c r="B69" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C69">
         <v>7</v>
@@ -2496,10 +2908,10 @@
         <v>0</v>
       </c>
       <c r="F69" s="2">
-        <v>44417</v>
+        <v>44451</v>
       </c>
       <c r="G69" t="s">
-        <v>157</v>
+        <v>222</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2507,7 +2919,7 @@
         <v>7</v>
       </c>
       <c r="B70" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C70">
         <v>7</v>
@@ -2519,10 +2931,10 @@
         <v>0</v>
       </c>
       <c r="F70" s="2">
-        <v>44234</v>
+        <v>44417</v>
       </c>
       <c r="G70" t="s">
-        <v>158</v>
+        <v>223</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2530,7 +2942,7 @@
         <v>7</v>
       </c>
       <c r="B71" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C71">
         <v>7</v>
@@ -2542,10 +2954,10 @@
         <v>0</v>
       </c>
       <c r="F71" s="2">
-        <v>44228</v>
+        <v>44234</v>
       </c>
       <c r="G71" t="s">
-        <v>159</v>
+        <v>224</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2553,7 +2965,7 @@
         <v>7</v>
       </c>
       <c r="B72" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C72">
         <v>8</v>
@@ -2565,10 +2977,10 @@
         <v>0</v>
       </c>
       <c r="F72" s="2">
-        <v>44246</v>
+        <v>44510</v>
       </c>
       <c r="G72" t="s">
-        <v>160</v>
+        <v>225</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2576,7 +2988,7 @@
         <v>7</v>
       </c>
       <c r="B73" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C73">
         <v>8</v>
@@ -2588,10 +3000,10 @@
         <v>0</v>
       </c>
       <c r="F73" s="2">
-        <v>44443</v>
+        <v>44228</v>
       </c>
       <c r="G73" t="s">
-        <v>161</v>
+        <v>226</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2599,22 +3011,22 @@
         <v>7</v>
       </c>
       <c r="B74" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C74">
         <v>8</v>
       </c>
       <c r="D74">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E74">
         <v>0</v>
       </c>
       <c r="F74" s="2">
-        <v>44201</v>
+        <v>44246</v>
       </c>
       <c r="G74" t="s">
-        <v>162</v>
+        <v>227</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2622,7 +3034,7 @@
         <v>7</v>
       </c>
       <c r="B75" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C75">
         <v>8</v>
@@ -2634,10 +3046,10 @@
         <v>0</v>
       </c>
       <c r="F75" s="2">
-        <v>44388</v>
+        <v>44443</v>
       </c>
       <c r="G75" t="s">
-        <v>79</v>
+        <v>228</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2645,22 +3057,22 @@
         <v>7</v>
       </c>
       <c r="B76" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="C76">
         <v>8</v>
       </c>
       <c r="D76">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E76">
         <v>0</v>
       </c>
       <c r="F76" s="2">
-        <v>44453</v>
+        <v>44201</v>
       </c>
       <c r="G76" t="s">
-        <v>92</v>
+        <v>229</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2668,7 +3080,7 @@
         <v>7</v>
       </c>
       <c r="B77" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C77">
         <v>8</v>
@@ -2680,10 +3092,10 @@
         <v>0</v>
       </c>
       <c r="F77" s="2">
-        <v>44254</v>
+        <v>44388</v>
       </c>
       <c r="G77" t="s">
-        <v>163</v>
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2691,7 +3103,7 @@
         <v>7</v>
       </c>
       <c r="B78" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="C78">
         <v>8</v>
@@ -2703,10 +3115,10 @@
         <v>0</v>
       </c>
       <c r="F78" s="2">
-        <v>44431</v>
+        <v>44453</v>
       </c>
       <c r="G78" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2714,7 +3126,7 @@
         <v>7</v>
       </c>
       <c r="B79" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C79">
         <v>8</v>
@@ -2726,10 +3138,10 @@
         <v>0</v>
       </c>
       <c r="F79" s="2">
-        <v>44437</v>
+        <v>44254</v>
       </c>
       <c r="G79" t="s">
-        <v>165</v>
+        <v>230</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2737,7 +3149,7 @@
         <v>7</v>
       </c>
       <c r="B80" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C80">
         <v>8</v>
@@ -2749,10 +3161,10 @@
         <v>0</v>
       </c>
       <c r="F80" s="2">
-        <v>44258</v>
+        <v>44431</v>
       </c>
       <c r="G80" t="s">
-        <v>166</v>
+        <v>231</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2760,7 +3172,7 @@
         <v>7</v>
       </c>
       <c r="B81" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C81">
         <v>8</v>
@@ -2772,10 +3184,10 @@
         <v>0</v>
       </c>
       <c r="F81" s="2">
-        <v>44356</v>
+        <v>44437</v>
       </c>
       <c r="G81" t="s">
-        <v>167</v>
+        <v>232</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2783,7 +3195,7 @@
         <v>7</v>
       </c>
       <c r="B82" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="C82">
         <v>9</v>
@@ -2795,10 +3207,10 @@
         <v>0</v>
       </c>
       <c r="F82" s="2">
-        <v>44436</v>
+        <v>44258</v>
       </c>
       <c r="G82" t="s">
-        <v>168</v>
+        <v>233</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2806,7 +3218,7 @@
         <v>7</v>
       </c>
       <c r="B83" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C83">
         <v>9</v>
@@ -2818,10 +3230,10 @@
         <v>0</v>
       </c>
       <c r="F83" s="2">
-        <v>44400</v>
+        <v>44356</v>
       </c>
       <c r="G83" t="s">
-        <v>169</v>
+        <v>234</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2829,7 +3241,7 @@
         <v>7</v>
       </c>
       <c r="B84" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C84">
         <v>9</v>
@@ -2841,10 +3253,10 @@
         <v>0</v>
       </c>
       <c r="F84" s="2">
-        <v>44294</v>
+        <v>44436</v>
       </c>
       <c r="G84" t="s">
-        <v>170</v>
+        <v>235</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2852,7 +3264,7 @@
         <v>7</v>
       </c>
       <c r="B85" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C85">
         <v>9</v>
@@ -2864,10 +3276,10 @@
         <v>0</v>
       </c>
       <c r="F85" s="2">
-        <v>44444</v>
+        <v>44400</v>
       </c>
       <c r="G85" t="s">
-        <v>171</v>
+        <v>236</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2875,7 +3287,7 @@
         <v>7</v>
       </c>
       <c r="B86" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="C86">
         <v>9</v>
@@ -2887,10 +3299,10 @@
         <v>0</v>
       </c>
       <c r="F86" s="2">
-        <v>44415</v>
+        <v>44294</v>
       </c>
       <c r="G86" t="s">
-        <v>172</v>
+        <v>237</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2898,7 +3310,7 @@
         <v>7</v>
       </c>
       <c r="B87" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C87">
         <v>9</v>
@@ -2910,10 +3322,10 @@
         <v>0</v>
       </c>
       <c r="F87" s="2">
-        <v>44241</v>
+        <v>44444</v>
       </c>
       <c r="G87" t="s">
-        <v>173</v>
+        <v>238</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2921,7 +3333,7 @@
         <v>7</v>
       </c>
       <c r="B88" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C88">
         <v>9</v>
@@ -2933,10 +3345,10 @@
         <v>0</v>
       </c>
       <c r="F88" s="2">
-        <v>44262</v>
+        <v>44415</v>
       </c>
       <c r="G88" t="s">
-        <v>174</v>
+        <v>239</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2944,7 +3356,7 @@
         <v>7</v>
       </c>
       <c r="B89" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C89">
         <v>9</v>
@@ -2956,10 +3368,10 @@
         <v>0</v>
       </c>
       <c r="F89" s="2">
-        <v>44245</v>
+        <v>44241</v>
       </c>
       <c r="G89" t="s">
-        <v>175</v>
+        <v>240</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2967,7 +3379,7 @@
         <v>7</v>
       </c>
       <c r="B90" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C90">
         <v>9</v>
@@ -2979,10 +3391,10 @@
         <v>0</v>
       </c>
       <c r="F90" s="2">
-        <v>44369</v>
+        <v>44262</v>
       </c>
       <c r="G90" t="s">
-        <v>176</v>
+        <v>241</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2990,7 +3402,7 @@
         <v>7</v>
       </c>
       <c r="B91" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C91">
         <v>9</v>
@@ -3002,10 +3414,1666 @@
         <v>0</v>
       </c>
       <c r="F91" s="2">
-        <v>44489</v>
+        <v>44245</v>
       </c>
       <c r="G91" t="s">
-        <v>177</v>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" t="s">
+        <v>8</v>
+      </c>
+      <c r="B92" t="s">
+        <v>95</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92">
+        <v>5</v>
+      </c>
+      <c r="E92">
+        <v>22</v>
+      </c>
+      <c r="F92" s="2">
+        <v>44457</v>
+      </c>
+      <c r="G92" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" t="s">
+        <v>8</v>
+      </c>
+      <c r="B93" t="s">
+        <v>96</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>5</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+      <c r="F93" s="2">
+        <v>44483</v>
+      </c>
+      <c r="G93" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" t="s">
+        <v>8</v>
+      </c>
+      <c r="B94" t="s">
+        <v>97</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>5</v>
+      </c>
+      <c r="E94">
+        <v>1</v>
+      </c>
+      <c r="F94" s="2">
+        <v>44460</v>
+      </c>
+      <c r="G94" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" t="s">
+        <v>8</v>
+      </c>
+      <c r="B95" t="s">
+        <v>55</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>5</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95" s="2">
+        <v>44501</v>
+      </c>
+      <c r="G95" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" t="s">
+        <v>8</v>
+      </c>
+      <c r="B96" t="s">
+        <v>98</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>5</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96" s="2">
+        <v>44491</v>
+      </c>
+      <c r="G96" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" t="s">
+        <v>8</v>
+      </c>
+      <c r="B97" t="s">
+        <v>99</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>5</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97" s="2">
+        <v>44445</v>
+      </c>
+      <c r="G97" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" t="s">
+        <v>8</v>
+      </c>
+      <c r="B98" t="s">
+        <v>100</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98" s="2">
+        <v>44511</v>
+      </c>
+      <c r="G98" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99" t="s">
+        <v>101</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99">
+        <v>5</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99" s="2">
+        <v>44502</v>
+      </c>
+      <c r="G99" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" t="s">
+        <v>8</v>
+      </c>
+      <c r="B100" t="s">
+        <v>102</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100">
+        <v>5</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100" s="2">
+        <v>44472</v>
+      </c>
+      <c r="G100" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" t="s">
+        <v>8</v>
+      </c>
+      <c r="B101" t="s">
+        <v>103</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <v>5</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101" s="2">
+        <v>44495</v>
+      </c>
+      <c r="G101" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" t="s">
+        <v>8</v>
+      </c>
+      <c r="B102" t="s">
+        <v>104</v>
+      </c>
+      <c r="C102">
+        <v>2</v>
+      </c>
+      <c r="D102">
+        <v>5</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102" s="2">
+        <v>44481</v>
+      </c>
+      <c r="G102" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" t="s">
+        <v>8</v>
+      </c>
+      <c r="B103" t="s">
+        <v>105</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
+      </c>
+      <c r="D103">
+        <v>5</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103" s="2">
+        <v>44470</v>
+      </c>
+      <c r="G103" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" t="s">
+        <v>8</v>
+      </c>
+      <c r="B104" t="s">
+        <v>106</v>
+      </c>
+      <c r="C104">
+        <v>2</v>
+      </c>
+      <c r="D104">
+        <v>5</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104" s="2">
+        <v>44500</v>
+      </c>
+      <c r="G104" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" t="s">
+        <v>8</v>
+      </c>
+      <c r="B105" t="s">
+        <v>107</v>
+      </c>
+      <c r="C105">
+        <v>2</v>
+      </c>
+      <c r="D105">
+        <v>1</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105" s="2">
+        <v>44506</v>
+      </c>
+      <c r="G105" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" t="s">
+        <v>8</v>
+      </c>
+      <c r="B106" t="s">
+        <v>108</v>
+      </c>
+      <c r="C106">
+        <v>2</v>
+      </c>
+      <c r="D106">
+        <v>5</v>
+      </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="F106" s="2">
+        <v>44478</v>
+      </c>
+      <c r="G106" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" t="s">
+        <v>8</v>
+      </c>
+      <c r="B107" t="s">
+        <v>62</v>
+      </c>
+      <c r="C107">
+        <v>2</v>
+      </c>
+      <c r="D107">
+        <v>5</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="F107" s="2">
+        <v>44469</v>
+      </c>
+      <c r="G107" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" t="s">
+        <v>8</v>
+      </c>
+      <c r="B108" t="s">
+        <v>109</v>
+      </c>
+      <c r="C108">
+        <v>2</v>
+      </c>
+      <c r="D108">
+        <v>5</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108" s="2">
+        <v>44443</v>
+      </c>
+      <c r="G108" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" t="s">
+        <v>8</v>
+      </c>
+      <c r="B109" t="s">
+        <v>110</v>
+      </c>
+      <c r="C109">
+        <v>2</v>
+      </c>
+      <c r="D109">
+        <v>5</v>
+      </c>
+      <c r="E109">
+        <v>0</v>
+      </c>
+      <c r="F109" s="2">
+        <v>44469</v>
+      </c>
+      <c r="G109" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" t="s">
+        <v>8</v>
+      </c>
+      <c r="B110" t="s">
+        <v>111</v>
+      </c>
+      <c r="C110">
+        <v>2</v>
+      </c>
+      <c r="D110">
+        <v>4</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="F110" s="2">
+        <v>44476</v>
+      </c>
+      <c r="G110" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" t="s">
+        <v>8</v>
+      </c>
+      <c r="B111" t="s">
+        <v>112</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
+      </c>
+      <c r="D111">
+        <v>5</v>
+      </c>
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="F111" s="2">
+        <v>44451</v>
+      </c>
+      <c r="G111" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" t="s">
+        <v>9</v>
+      </c>
+      <c r="B112" t="s">
+        <v>113</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+      <c r="D112">
+        <v>5</v>
+      </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112" s="2">
+        <v>44447</v>
+      </c>
+      <c r="G112" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" t="s">
+        <v>9</v>
+      </c>
+      <c r="B113" t="s">
+        <v>55</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="D113">
+        <v>5</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113" s="2">
+        <v>44421</v>
+      </c>
+      <c r="G113" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" t="s">
+        <v>9</v>
+      </c>
+      <c r="B114" t="s">
+        <v>114</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
+      </c>
+      <c r="D114">
+        <v>5</v>
+      </c>
+      <c r="E114">
+        <v>0</v>
+      </c>
+      <c r="F114" s="2">
+        <v>44495</v>
+      </c>
+      <c r="G114" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" t="s">
+        <v>9</v>
+      </c>
+      <c r="B115" t="s">
+        <v>115</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+      <c r="D115">
+        <v>5</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="F115" s="2">
+        <v>44500</v>
+      </c>
+      <c r="G115" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
+      <c r="A116" t="s">
+        <v>9</v>
+      </c>
+      <c r="B116" t="s">
+        <v>116</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116">
+        <v>5</v>
+      </c>
+      <c r="E116">
+        <v>0</v>
+      </c>
+      <c r="F116" s="2">
+        <v>44482</v>
+      </c>
+      <c r="G116" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
+      <c r="A117" t="s">
+        <v>9</v>
+      </c>
+      <c r="B117" t="s">
+        <v>55</v>
+      </c>
+      <c r="C117">
+        <v>1</v>
+      </c>
+      <c r="D117">
+        <v>5</v>
+      </c>
+      <c r="E117">
+        <v>0</v>
+      </c>
+      <c r="F117" s="2">
+        <v>44490</v>
+      </c>
+      <c r="G117" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="A118" t="s">
+        <v>9</v>
+      </c>
+      <c r="B118" t="s">
+        <v>117</v>
+      </c>
+      <c r="C118">
+        <v>1</v>
+      </c>
+      <c r="D118">
+        <v>5</v>
+      </c>
+      <c r="E118">
+        <v>0</v>
+      </c>
+      <c r="F118" s="2">
+        <v>44485</v>
+      </c>
+      <c r="G118" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
+      <c r="A119" t="s">
+        <v>9</v>
+      </c>
+      <c r="B119" t="s">
+        <v>118</v>
+      </c>
+      <c r="C119">
+        <v>1</v>
+      </c>
+      <c r="D119">
+        <v>4</v>
+      </c>
+      <c r="E119">
+        <v>0</v>
+      </c>
+      <c r="F119" s="2">
+        <v>44487</v>
+      </c>
+      <c r="G119" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" t="s">
+        <v>9</v>
+      </c>
+      <c r="B120" t="s">
+        <v>119</v>
+      </c>
+      <c r="C120">
+        <v>1</v>
+      </c>
+      <c r="D120">
+        <v>5</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120" s="2">
+        <v>44412</v>
+      </c>
+      <c r="G120" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" t="s">
+        <v>9</v>
+      </c>
+      <c r="B121" t="s">
+        <v>120</v>
+      </c>
+      <c r="C121">
+        <v>1</v>
+      </c>
+      <c r="D121">
+        <v>5</v>
+      </c>
+      <c r="E121">
+        <v>0</v>
+      </c>
+      <c r="F121" s="2">
+        <v>44500</v>
+      </c>
+      <c r="G121" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" t="s">
+        <v>9</v>
+      </c>
+      <c r="B122" t="s">
+        <v>121</v>
+      </c>
+      <c r="C122">
+        <v>2</v>
+      </c>
+      <c r="D122">
+        <v>5</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="F122" s="2">
+        <v>44473</v>
+      </c>
+      <c r="G122" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="A123" t="s">
+        <v>9</v>
+      </c>
+      <c r="B123" t="s">
+        <v>59</v>
+      </c>
+      <c r="C123">
+        <v>2</v>
+      </c>
+      <c r="D123">
+        <v>5</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="F123" s="2">
+        <v>44507</v>
+      </c>
+      <c r="G123" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" t="s">
+        <v>9</v>
+      </c>
+      <c r="B124" t="s">
+        <v>122</v>
+      </c>
+      <c r="C124">
+        <v>2</v>
+      </c>
+      <c r="D124">
+        <v>5</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+      <c r="F124" s="2">
+        <v>44434</v>
+      </c>
+      <c r="G124" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
+      <c r="A125" t="s">
+        <v>9</v>
+      </c>
+      <c r="B125" t="s">
+        <v>123</v>
+      </c>
+      <c r="C125">
+        <v>2</v>
+      </c>
+      <c r="D125">
+        <v>5</v>
+      </c>
+      <c r="E125">
+        <v>0</v>
+      </c>
+      <c r="F125" s="2">
+        <v>44447</v>
+      </c>
+      <c r="G125" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
+      <c r="A126" t="s">
+        <v>9</v>
+      </c>
+      <c r="B126" t="s">
+        <v>59</v>
+      </c>
+      <c r="C126">
+        <v>2</v>
+      </c>
+      <c r="D126">
+        <v>5</v>
+      </c>
+      <c r="E126">
+        <v>0</v>
+      </c>
+      <c r="F126" s="2">
+        <v>44417</v>
+      </c>
+      <c r="G126" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
+      <c r="A127" t="s">
+        <v>9</v>
+      </c>
+      <c r="B127" t="s">
+        <v>124</v>
+      </c>
+      <c r="C127">
+        <v>2</v>
+      </c>
+      <c r="D127">
+        <v>5</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+      <c r="F127" s="2">
+        <v>44509</v>
+      </c>
+      <c r="G127" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
+      <c r="A128" t="s">
+        <v>9</v>
+      </c>
+      <c r="B128" t="s">
+        <v>58</v>
+      </c>
+      <c r="C128">
+        <v>2</v>
+      </c>
+      <c r="D128">
+        <v>5</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="F128" s="2">
+        <v>44480</v>
+      </c>
+      <c r="G128" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
+      <c r="A129" t="s">
+        <v>9</v>
+      </c>
+      <c r="B129" t="s">
+        <v>109</v>
+      </c>
+      <c r="C129">
+        <v>2</v>
+      </c>
+      <c r="D129">
+        <v>5</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="F129" s="2">
+        <v>44412</v>
+      </c>
+      <c r="G129" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
+      <c r="A130" t="s">
+        <v>9</v>
+      </c>
+      <c r="B130" t="s">
+        <v>125</v>
+      </c>
+      <c r="C130">
+        <v>2</v>
+      </c>
+      <c r="D130">
+        <v>5</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="F130" s="2">
+        <v>44509</v>
+      </c>
+      <c r="G130" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" t="s">
+        <v>9</v>
+      </c>
+      <c r="B131" t="s">
+        <v>126</v>
+      </c>
+      <c r="C131">
+        <v>2</v>
+      </c>
+      <c r="D131">
+        <v>5</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
+      <c r="F131" s="2">
+        <v>44417</v>
+      </c>
+      <c r="G131" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
+      <c r="A132" t="s">
+        <v>9</v>
+      </c>
+      <c r="B132" t="s">
+        <v>51</v>
+      </c>
+      <c r="C132">
+        <v>3</v>
+      </c>
+      <c r="D132">
+        <v>4</v>
+      </c>
+      <c r="E132">
+        <v>0</v>
+      </c>
+      <c r="F132" s="2">
+        <v>44414</v>
+      </c>
+      <c r="G132" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
+      <c r="A133" t="s">
+        <v>9</v>
+      </c>
+      <c r="B133" t="s">
+        <v>127</v>
+      </c>
+      <c r="C133">
+        <v>3</v>
+      </c>
+      <c r="D133">
+        <v>5</v>
+      </c>
+      <c r="E133">
+        <v>0</v>
+      </c>
+      <c r="F133" s="2">
+        <v>44386</v>
+      </c>
+      <c r="G133" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
+      <c r="A134" t="s">
+        <v>9</v>
+      </c>
+      <c r="B134" t="s">
+        <v>128</v>
+      </c>
+      <c r="C134">
+        <v>3</v>
+      </c>
+      <c r="D134">
+        <v>4</v>
+      </c>
+      <c r="E134">
+        <v>0</v>
+      </c>
+      <c r="F134" s="2">
+        <v>44416</v>
+      </c>
+      <c r="G134" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
+      <c r="A135" t="s">
+        <v>9</v>
+      </c>
+      <c r="B135" t="s">
+        <v>129</v>
+      </c>
+      <c r="C135">
+        <v>3</v>
+      </c>
+      <c r="D135">
+        <v>5</v>
+      </c>
+      <c r="E135">
+        <v>2</v>
+      </c>
+      <c r="F135" s="2">
+        <v>44369</v>
+      </c>
+      <c r="G135" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7">
+      <c r="A136" t="s">
+        <v>9</v>
+      </c>
+      <c r="B136" t="s">
+        <v>130</v>
+      </c>
+      <c r="C136">
+        <v>3</v>
+      </c>
+      <c r="D136">
+        <v>5</v>
+      </c>
+      <c r="E136">
+        <v>2</v>
+      </c>
+      <c r="F136" s="2">
+        <v>44366</v>
+      </c>
+      <c r="G136" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7">
+      <c r="A137" t="s">
+        <v>9</v>
+      </c>
+      <c r="B137" t="s">
+        <v>131</v>
+      </c>
+      <c r="C137">
+        <v>3</v>
+      </c>
+      <c r="D137">
+        <v>5</v>
+      </c>
+      <c r="E137">
+        <v>1</v>
+      </c>
+      <c r="F137" s="2">
+        <v>44378</v>
+      </c>
+      <c r="G137" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7">
+      <c r="A138" t="s">
+        <v>9</v>
+      </c>
+      <c r="B138" t="s">
+        <v>132</v>
+      </c>
+      <c r="C138">
+        <v>3</v>
+      </c>
+      <c r="D138">
+        <v>5</v>
+      </c>
+      <c r="E138">
+        <v>1</v>
+      </c>
+      <c r="F138" s="2">
+        <v>44426</v>
+      </c>
+      <c r="G138" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7">
+      <c r="A139" t="s">
+        <v>9</v>
+      </c>
+      <c r="B139" t="s">
+        <v>133</v>
+      </c>
+      <c r="C139">
+        <v>3</v>
+      </c>
+      <c r="D139">
+        <v>4</v>
+      </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
+      <c r="F139" s="2">
+        <v>44426</v>
+      </c>
+      <c r="G139" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7">
+      <c r="A140" t="s">
+        <v>9</v>
+      </c>
+      <c r="B140" t="s">
+        <v>134</v>
+      </c>
+      <c r="C140">
+        <v>3</v>
+      </c>
+      <c r="D140">
+        <v>5</v>
+      </c>
+      <c r="E140">
+        <v>0</v>
+      </c>
+      <c r="F140" s="2">
+        <v>44404</v>
+      </c>
+      <c r="G140" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7">
+      <c r="A141" t="s">
+        <v>9</v>
+      </c>
+      <c r="B141" t="s">
+        <v>135</v>
+      </c>
+      <c r="C141">
+        <v>3</v>
+      </c>
+      <c r="D141">
+        <v>5</v>
+      </c>
+      <c r="E141">
+        <v>0</v>
+      </c>
+      <c r="F141" s="2">
+        <v>44406</v>
+      </c>
+      <c r="G141" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7">
+      <c r="A142" t="s">
+        <v>9</v>
+      </c>
+      <c r="B142" t="s">
+        <v>136</v>
+      </c>
+      <c r="C142">
+        <v>4</v>
+      </c>
+      <c r="D142">
+        <v>5</v>
+      </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
+      <c r="F142" s="2">
+        <v>44376</v>
+      </c>
+      <c r="G142" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7">
+      <c r="A143" t="s">
+        <v>9</v>
+      </c>
+      <c r="B143" t="s">
+        <v>137</v>
+      </c>
+      <c r="C143">
+        <v>4</v>
+      </c>
+      <c r="D143">
+        <v>5</v>
+      </c>
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="F143" s="2">
+        <v>44382</v>
+      </c>
+      <c r="G143" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7">
+      <c r="A144" t="s">
+        <v>9</v>
+      </c>
+      <c r="B144" t="s">
+        <v>138</v>
+      </c>
+      <c r="C144">
+        <v>4</v>
+      </c>
+      <c r="D144">
+        <v>5</v>
+      </c>
+      <c r="E144">
+        <v>0</v>
+      </c>
+      <c r="F144" s="2">
+        <v>44377</v>
+      </c>
+      <c r="G144" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
+      <c r="A145" t="s">
+        <v>9</v>
+      </c>
+      <c r="B145" t="s">
+        <v>139</v>
+      </c>
+      <c r="C145">
+        <v>4</v>
+      </c>
+      <c r="D145">
+        <v>4</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145" s="2">
+        <v>44492</v>
+      </c>
+      <c r="G145" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="A146" t="s">
+        <v>9</v>
+      </c>
+      <c r="B146" t="s">
+        <v>140</v>
+      </c>
+      <c r="C146">
+        <v>4</v>
+      </c>
+      <c r="D146">
+        <v>5</v>
+      </c>
+      <c r="E146">
+        <v>0</v>
+      </c>
+      <c r="F146" s="2">
+        <v>44384</v>
+      </c>
+      <c r="G146" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7">
+      <c r="A147" t="s">
+        <v>9</v>
+      </c>
+      <c r="B147" t="s">
+        <v>141</v>
+      </c>
+      <c r="C147">
+        <v>4</v>
+      </c>
+      <c r="D147">
+        <v>5</v>
+      </c>
+      <c r="E147">
+        <v>0</v>
+      </c>
+      <c r="F147" s="2">
+        <v>44368</v>
+      </c>
+      <c r="G147" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
+      <c r="A148" t="s">
+        <v>9</v>
+      </c>
+      <c r="B148" t="s">
+        <v>142</v>
+      </c>
+      <c r="C148">
+        <v>4</v>
+      </c>
+      <c r="D148">
+        <v>5</v>
+      </c>
+      <c r="E148">
+        <v>0</v>
+      </c>
+      <c r="F148" s="2">
+        <v>44368</v>
+      </c>
+      <c r="G148" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7">
+      <c r="A149" t="s">
+        <v>9</v>
+      </c>
+      <c r="B149" t="s">
+        <v>143</v>
+      </c>
+      <c r="C149">
+        <v>4</v>
+      </c>
+      <c r="D149">
+        <v>5</v>
+      </c>
+      <c r="E149">
+        <v>0</v>
+      </c>
+      <c r="F149" s="2">
+        <v>44401</v>
+      </c>
+      <c r="G149" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
+      <c r="A150" t="s">
+        <v>9</v>
+      </c>
+      <c r="B150" t="s">
+        <v>144</v>
+      </c>
+      <c r="C150">
+        <v>4</v>
+      </c>
+      <c r="D150">
+        <v>5</v>
+      </c>
+      <c r="E150">
+        <v>0</v>
+      </c>
+      <c r="F150" s="2">
+        <v>44384</v>
+      </c>
+      <c r="G150" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7">
+      <c r="A151" t="s">
+        <v>9</v>
+      </c>
+      <c r="B151" t="s">
+        <v>145</v>
+      </c>
+      <c r="C151">
+        <v>4</v>
+      </c>
+      <c r="D151">
+        <v>5</v>
+      </c>
+      <c r="E151">
+        <v>0</v>
+      </c>
+      <c r="F151" s="2">
+        <v>44373</v>
+      </c>
+      <c r="G151" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7">
+      <c r="A152" t="s">
+        <v>9</v>
+      </c>
+      <c r="B152" t="s">
+        <v>146</v>
+      </c>
+      <c r="C152">
+        <v>5</v>
+      </c>
+      <c r="D152">
+        <v>5</v>
+      </c>
+      <c r="E152">
+        <v>0</v>
+      </c>
+      <c r="F152" s="2">
+        <v>44390</v>
+      </c>
+      <c r="G152" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7">
+      <c r="A153" t="s">
+        <v>9</v>
+      </c>
+      <c r="B153" t="s">
+        <v>147</v>
+      </c>
+      <c r="C153">
+        <v>5</v>
+      </c>
+      <c r="D153">
+        <v>5</v>
+      </c>
+      <c r="E153">
+        <v>0</v>
+      </c>
+      <c r="F153" s="2">
+        <v>44440</v>
+      </c>
+      <c r="G153" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7">
+      <c r="A154" t="s">
+        <v>9</v>
+      </c>
+      <c r="B154" t="s">
+        <v>148</v>
+      </c>
+      <c r="C154">
+        <v>5</v>
+      </c>
+      <c r="D154">
+        <v>5</v>
+      </c>
+      <c r="E154">
+        <v>0</v>
+      </c>
+      <c r="F154" s="2">
+        <v>44377</v>
+      </c>
+      <c r="G154" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7">
+      <c r="A155" t="s">
+        <v>9</v>
+      </c>
+      <c r="B155" t="s">
+        <v>149</v>
+      </c>
+      <c r="C155">
+        <v>5</v>
+      </c>
+      <c r="D155">
+        <v>5</v>
+      </c>
+      <c r="E155">
+        <v>0</v>
+      </c>
+      <c r="F155" s="2">
+        <v>44376</v>
+      </c>
+      <c r="G155" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7">
+      <c r="A156" t="s">
+        <v>9</v>
+      </c>
+      <c r="B156" t="s">
+        <v>150</v>
+      </c>
+      <c r="C156">
+        <v>5</v>
+      </c>
+      <c r="D156">
+        <v>5</v>
+      </c>
+      <c r="E156">
+        <v>0</v>
+      </c>
+      <c r="F156" s="2">
+        <v>44444</v>
+      </c>
+      <c r="G156" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7">
+      <c r="A157" t="s">
+        <v>9</v>
+      </c>
+      <c r="B157" t="s">
+        <v>151</v>
+      </c>
+      <c r="C157">
+        <v>5</v>
+      </c>
+      <c r="D157">
+        <v>5</v>
+      </c>
+      <c r="E157">
+        <v>0</v>
+      </c>
+      <c r="F157" s="2">
+        <v>44393</v>
+      </c>
+      <c r="G157" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7">
+      <c r="A158" t="s">
+        <v>9</v>
+      </c>
+      <c r="B158" t="s">
+        <v>152</v>
+      </c>
+      <c r="C158">
+        <v>5</v>
+      </c>
+      <c r="D158">
+        <v>5</v>
+      </c>
+      <c r="E158">
+        <v>0</v>
+      </c>
+      <c r="F158" s="2">
+        <v>44387</v>
+      </c>
+      <c r="G158" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7">
+      <c r="A159" t="s">
+        <v>9</v>
+      </c>
+      <c r="B159" t="s">
+        <v>153</v>
+      </c>
+      <c r="C159">
+        <v>5</v>
+      </c>
+      <c r="D159">
+        <v>4</v>
+      </c>
+      <c r="E159">
+        <v>0</v>
+      </c>
+      <c r="F159" s="2">
+        <v>44456</v>
+      </c>
+      <c r="G159" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7">
+      <c r="A160" t="s">
+        <v>9</v>
+      </c>
+      <c r="B160" t="s">
+        <v>154</v>
+      </c>
+      <c r="C160">
+        <v>5</v>
+      </c>
+      <c r="D160">
+        <v>4</v>
+      </c>
+      <c r="E160">
+        <v>0</v>
+      </c>
+      <c r="F160" s="2">
+        <v>44416</v>
+      </c>
+      <c r="G160" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7">
+      <c r="A161" t="s">
+        <v>9</v>
+      </c>
+      <c r="B161" t="s">
+        <v>155</v>
+      </c>
+      <c r="C161">
+        <v>5</v>
+      </c>
+      <c r="D161">
+        <v>5</v>
+      </c>
+      <c r="E161">
+        <v>0</v>
+      </c>
+      <c r="F161" s="2">
+        <v>44371</v>
+      </c>
+      <c r="G161" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7">
+      <c r="A162" t="s">
+        <v>9</v>
+      </c>
+      <c r="B162" t="s">
+        <v>156</v>
+      </c>
+      <c r="C162">
+        <v>6</v>
+      </c>
+      <c r="D162">
+        <v>5</v>
+      </c>
+      <c r="E162">
+        <v>0</v>
+      </c>
+      <c r="F162" s="2">
+        <v>44454</v>
+      </c>
+      <c r="G162" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7">
+      <c r="A163" t="s">
+        <v>9</v>
+      </c>
+      <c r="B163" t="s">
+        <v>157</v>
+      </c>
+      <c r="C163">
+        <v>6</v>
+      </c>
+      <c r="D163">
+        <v>5</v>
+      </c>
+      <c r="E163">
+        <v>0</v>
+      </c>
+      <c r="F163" s="2">
+        <v>44512</v>
+      </c>
+      <c r="G163" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>